<commit_message>
minor bugfix BOM: WAS2, WAS3
</commit_message>
<xml_diff>
--- a/central_unit/production_data/BOM_Central Unit for AgOpenGPS__Shenzhen2u .xlsx
+++ b/central_unit/production_data/BOM_Central Unit for AgOpenGPS__Shenzhen2u .xlsx
@@ -425,7 +425,7 @@
     <t xml:space="preserve">CC0603JRX7R8BB104</t>
   </si>
   <si>
-    <t xml:space="preserve">REMOTE,M1,CHA,WAS1,STEER,WORK</t>
+    <t xml:space="preserve">REMOTE,M1,CHA,WAS2,STEER,WORK</t>
   </si>
   <si>
     <t xml:space="preserve">Everlight Elec</t>
@@ -590,7 +590,7 @@
     <t xml:space="preserve">USB-C-SMD_KH-TYPE-C-16P</t>
   </si>
   <si>
-    <t xml:space="preserve">CHB,WAS2,M2</t>
+    <t xml:space="preserve">CHB,WAS3,M2</t>
   </si>
   <si>
     <t xml:space="preserve">NATIONSTAR</t>
@@ -801,13 +801,12 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="4">
+  <numFmts count="3">
     <numFmt numFmtId="164" formatCode="General"/>
-    <numFmt numFmtId="165" formatCode="#,##0.00\ [$€-407];[RED]\-#,##0.00\ [$€-407]"/>
-    <numFmt numFmtId="166" formatCode="0.00"/>
-    <numFmt numFmtId="167" formatCode="0;;;@"/>
+    <numFmt numFmtId="165" formatCode="0.00"/>
+    <numFmt numFmtId="166" formatCode="0;;;@"/>
   </numFmts>
-  <fonts count="32">
+  <fonts count="29">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
@@ -828,19 +827,6 @@
       <sz val="10"/>
       <name val="Arial"/>
       <family val="0"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <name val="Mangal"/>
-      <family val="2"/>
-      <charset val="1"/>
-    </font>
-    <font>
-      <u val="single"/>
-      <sz val="10"/>
-      <name val="Mangal"/>
-      <family val="2"/>
-      <charset val="1"/>
     </font>
     <font>
       <sz val="10"/>
@@ -1016,13 +1002,7 @@
       <sz val="10"/>
       <color rgb="FF15AF3D"/>
       <name val="Nirmala UI"/>
-      <family val="2"/>
-    </font>
-    <font>
-      <sz val="12"/>
-      <color rgb="FF000000"/>
-      <name val="Calibri"/>
-      <family val="2"/>
+      <family val="0"/>
     </font>
     <font>
       <sz val="9"/>
@@ -1159,7 +1139,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="25">
+  <cellStyleXfs count="21">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -1183,311 +1163,283 @@
     <xf numFmtId="44" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="164" fontId="14" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="bottom" textRotation="90" wrapText="false" indent="0" shrinkToFit="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-    </xf>
-    <xf numFmtId="165" fontId="5" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="12" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="69">
+  <cellXfs count="66">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="true">
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="164" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="right" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="164" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="left" vertical="top" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="164" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="left" vertical="top" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="164" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="right" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="11" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="164" fontId="9" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="164" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="15" fillId="0" borderId="0" xfId="20" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="164" fontId="13" fillId="0" borderId="0" xfId="20" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="left" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="164" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="right" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="14" fillId="0" borderId="0" xfId="20" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="164" fontId="12" fillId="0" borderId="0" xfId="20" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="left" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="164" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="left" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="17" fillId="2" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="15" fillId="2" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="18" fillId="2" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="16" fillId="2" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="18" fillId="2" borderId="3" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="16" fillId="2" borderId="3" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="18" fillId="2" borderId="3" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="16" fillId="2" borderId="3" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="18" fillId="0" borderId="4" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="16" fillId="0" borderId="4" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="19" fillId="3" borderId="5" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="17" fillId="3" borderId="5" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="20" fillId="3" borderId="5" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="18" fillId="3" borderId="5" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="20" fillId="3" borderId="6" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="18" fillId="3" borderId="6" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="18" fillId="0" borderId="4" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="16" fillId="0" borderId="4" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="21" fillId="0" borderId="5" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="19" fillId="0" borderId="5" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="6" fillId="0" borderId="5" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="5" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="6" fillId="0" borderId="6" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="6" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="19" fillId="3" borderId="7" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="17" fillId="3" borderId="7" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="20" fillId="3" borderId="7" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="18" fillId="3" borderId="7" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="20" fillId="3" borderId="8" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="18" fillId="3" borderId="8" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="21" fillId="0" borderId="7" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="19" fillId="0" borderId="7" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="6" fillId="0" borderId="7" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="7" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="6" fillId="0" borderId="8" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="8" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="22" fillId="3" borderId="5" xfId="20" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="164" fontId="20" fillId="3" borderId="5" xfId="20" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="21" fillId="2" borderId="9" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="17" fillId="3" borderId="9" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="top" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="9" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="top" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="top" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="21" fillId="2" borderId="9" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="17" fillId="3" borderId="9" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="9" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="3" borderId="9" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="left" vertical="top" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="left" vertical="top" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="left" vertical="top" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="165" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="22" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+    <xf numFmtId="164" fontId="23" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="23" fillId="2" borderId="9" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+    <xf numFmtId="164" fontId="24" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="19" fillId="3" borderId="9" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="top" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+    <xf numFmtId="165" fontId="22" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="6" fillId="0" borderId="9" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="top" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+    <xf numFmtId="164" fontId="23" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="top" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+    <xf numFmtId="164" fontId="25" fillId="2" borderId="9" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+    <xf numFmtId="164" fontId="25" fillId="2" borderId="9" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="right" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="23" fillId="2" borderId="9" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="26" fillId="3" borderId="9" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="19" fillId="3" borderId="9" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="6" fillId="0" borderId="9" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="6" fillId="3" borderId="9" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="left" vertical="top" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="left" vertical="top" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="left" vertical="top" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="left" vertical="top" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="166" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="24" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="25" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="26" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="166" fontId="24" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="25" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="27" fillId="2" borderId="9" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="27" fillId="2" borderId="9" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="right" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="28" fillId="3" borderId="9" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="28" fillId="3" borderId="9" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="26" fillId="3" borderId="9" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="28" fillId="3" borderId="9" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="26" fillId="3" borderId="9" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="167" fontId="10" fillId="0" borderId="9" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="166" fontId="8" fillId="0" borderId="9" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
   </cellXfs>
-  <cellStyles count="11">
+  <cellStyles count="7">
     <cellStyle name="Normal" xfId="0" builtinId="0" customBuiltin="false"/>
     <cellStyle name="Comma" xfId="15" builtinId="3" customBuiltin="false"/>
     <cellStyle name="Comma [0]" xfId="16" builtinId="6" customBuiltin="false"/>
     <cellStyle name="Currency" xfId="17" builtinId="4" customBuiltin="false"/>
     <cellStyle name="Currency [0]" xfId="18" builtinId="7" customBuiltin="false"/>
     <cellStyle name="Percent" xfId="19" builtinId="5" customBuiltin="false"/>
-    <cellStyle name="Heading 1" xfId="21" builtinId="53" customBuiltin="true"/>
-    <cellStyle name="Heading1 2" xfId="22" builtinId="53" customBuiltin="true"/>
-    <cellStyle name="Result 3" xfId="23" builtinId="53" customBuiltin="true"/>
-    <cellStyle name="Result2 4" xfId="24" builtinId="53" customBuiltin="true"/>
     <cellStyle name="*unknown*" xfId="20" builtinId="8" customBuiltin="false"/>
   </cellStyles>
   <colors>
@@ -1564,9 +1516,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>4</xdr:col>
-      <xdr:colOff>923400</xdr:colOff>
+      <xdr:colOff>923040</xdr:colOff>
       <xdr:row>6</xdr:row>
-      <xdr:rowOff>97200</xdr:rowOff>
+      <xdr:rowOff>96840</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -1575,8 +1527,8 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="1819080" y="133200"/>
-          <a:ext cx="2285640" cy="1036800"/>
+          <a:off x="1790640" y="133200"/>
+          <a:ext cx="2265840" cy="1036440"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -1596,7 +1548,7 @@
         <a:bodyPr lIns="90000" rIns="90000" tIns="45000" bIns="45000"/>
         <a:p>
           <a:r>
-            <a:rPr b="1" lang="de-DE" sz="1000" spc="-1" strike="noStrike">
+            <a:rPr b="1" lang="en-GB" sz="1000" spc="-1" strike="noStrike">
               <a:solidFill>
                 <a:srgbClr val="15af3d"/>
               </a:solidFill>
@@ -1609,65 +1561,7 @@
             </a:rPr>
             <a:t>SHENZHEN2U LTD.</a:t>
           </a:r>
-          <a:r>
-            <a:rPr b="0" lang="de-DE" sz="1200" spc="-1" strike="noStrike">
-              <a:solidFill>
-                <a:srgbClr val="000000"/>
-              </a:solidFill>
-              <a:uFill>
-                <a:solidFill>
-                  <a:srgbClr val="ffffff"/>
-                </a:solidFill>
-              </a:uFill>
-              <a:latin typeface="Calibri"/>
-            </a:rPr>
-            <a:t>
-</a:t>
-          </a:r>
-          <a:r>
-            <a:rPr b="0" lang="de-DE" sz="900" spc="-1" strike="noStrike">
-              <a:solidFill>
-                <a:srgbClr val="000000"/>
-              </a:solidFill>
-              <a:uFill>
-                <a:solidFill>
-                  <a:srgbClr val="ffffff"/>
-                </a:solidFill>
-              </a:uFill>
-              <a:latin typeface="Calibri Light"/>
-            </a:rPr>
-            <a:t>Unit 04, 7/F Bright Way Tower No. 33 </a:t>
-          </a:r>
-          <a:r>
-            <a:rPr b="0" lang="de-DE" sz="900" spc="-1" strike="noStrike">
-              <a:solidFill>
-                <a:srgbClr val="000000"/>
-              </a:solidFill>
-              <a:uFill>
-                <a:solidFill>
-                  <a:srgbClr val="ffffff"/>
-                </a:solidFill>
-              </a:uFill>
-              <a:latin typeface="Calibri Light"/>
-            </a:rPr>
-            <a:t>
-</a:t>
-          </a:r>
-          <a:r>
-            <a:rPr b="0" lang="de-DE" sz="900" spc="-1" strike="noStrike">
-              <a:solidFill>
-                <a:srgbClr val="000000"/>
-              </a:solidFill>
-              <a:uFill>
-                <a:solidFill>
-                  <a:srgbClr val="ffffff"/>
-                </a:solidFill>
-              </a:uFill>
-              <a:latin typeface="Calibri Light"/>
-            </a:rPr>
-            <a:t>Mong Kok Rd, Kowloon, Hong Kong </a:t>
-          </a:r>
-          <a:endParaRPr b="0" lang="de-DE" sz="1200" spc="-1" strike="noStrike">
+          <a:endParaRPr b="0" lang="en-GB" sz="1200" spc="-1" strike="noStrike">
             <a:solidFill>
               <a:srgbClr val="000000"/>
             </a:solidFill>
@@ -1681,7 +1575,61 @@
         </a:p>
         <a:p>
           <a:r>
-            <a:rPr b="0" lang="de-DE" sz="900" spc="-1" strike="noStrike">
+            <a:rPr b="0" lang="en-GB" sz="900" spc="-1" strike="noStrike">
+              <a:solidFill>
+                <a:srgbClr val="000000"/>
+              </a:solidFill>
+              <a:uFill>
+                <a:solidFill>
+                  <a:srgbClr val="ffffff"/>
+                </a:solidFill>
+              </a:uFill>
+              <a:latin typeface="Calibri Light"/>
+            </a:rPr>
+            <a:t>Unit 04, 7/F Bright Way Tower No. 33 </a:t>
+          </a:r>
+          <a:endParaRPr b="0" lang="en-GB" sz="1200" spc="-1" strike="noStrike">
+            <a:solidFill>
+              <a:srgbClr val="000000"/>
+            </a:solidFill>
+            <a:uFill>
+              <a:solidFill>
+                <a:srgbClr val="ffffff"/>
+              </a:solidFill>
+            </a:uFill>
+            <a:latin typeface="Times New Roman"/>
+          </a:endParaRPr>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr b="0" lang="en-GB" sz="900" spc="-1" strike="noStrike">
+              <a:solidFill>
+                <a:srgbClr val="000000"/>
+              </a:solidFill>
+              <a:uFill>
+                <a:solidFill>
+                  <a:srgbClr val="ffffff"/>
+                </a:solidFill>
+              </a:uFill>
+              <a:latin typeface="Calibri Light"/>
+            </a:rPr>
+            <a:t>Mong Kok Rd, Kowloon, Hong Kong </a:t>
+          </a:r>
+          <a:endParaRPr b="0" lang="en-GB" sz="1200" spc="-1" strike="noStrike">
+            <a:solidFill>
+              <a:srgbClr val="000000"/>
+            </a:solidFill>
+            <a:uFill>
+              <a:solidFill>
+                <a:srgbClr val="ffffff"/>
+              </a:solidFill>
+            </a:uFill>
+            <a:latin typeface="Times New Roman"/>
+          </a:endParaRPr>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr b="0" lang="en-GB" sz="900" spc="-1" strike="noStrike">
               <a:solidFill>
                 <a:srgbClr val="000000"/>
               </a:solidFill>
@@ -1694,23 +1642,21 @@
             </a:rPr>
             <a:t>info@shenzhen2u.com | +86 159 1919 2620</a:t>
           </a:r>
+          <a:endParaRPr b="0" lang="en-GB" sz="1200" spc="-1" strike="noStrike">
+            <a:solidFill>
+              <a:srgbClr val="000000"/>
+            </a:solidFill>
+            <a:uFill>
+              <a:solidFill>
+                <a:srgbClr val="ffffff"/>
+              </a:solidFill>
+            </a:uFill>
+            <a:latin typeface="Times New Roman"/>
+          </a:endParaRPr>
+        </a:p>
+        <a:p>
           <a:r>
-            <a:rPr b="0" lang="de-DE" sz="900" spc="-1" strike="noStrike">
-              <a:solidFill>
-                <a:srgbClr val="000000"/>
-              </a:solidFill>
-              <a:uFill>
-                <a:solidFill>
-                  <a:srgbClr val="ffffff"/>
-                </a:solidFill>
-              </a:uFill>
-              <a:latin typeface="Calibri Light"/>
-            </a:rPr>
-            <a:t>
-</a:t>
-          </a:r>
-          <a:r>
-            <a:rPr b="0" lang="de-DE" sz="900" spc="-1" strike="noStrike">
+            <a:rPr b="0" lang="en-GB" sz="900" spc="-1" strike="noStrike">
               <a:solidFill>
                 <a:srgbClr val="000000"/>
               </a:solidFill>
@@ -1723,7 +1669,7 @@
             </a:rPr>
             <a:t>www.shenzhen2u.com</a:t>
           </a:r>
-          <a:endParaRPr b="0" lang="de-DE" sz="1200" spc="-1" strike="noStrike">
+          <a:endParaRPr b="0" lang="en-GB" sz="1200" spc="-1" strike="noStrike">
             <a:solidFill>
               <a:srgbClr val="000000"/>
             </a:solidFill>
@@ -1748,9 +1694,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>2</xdr:col>
-      <xdr:colOff>578520</xdr:colOff>
+      <xdr:colOff>578160</xdr:colOff>
       <xdr:row>5</xdr:row>
-      <xdr:rowOff>130320</xdr:rowOff>
+      <xdr:rowOff>129960</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -1763,8 +1709,8 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="819000" y="123840"/>
-          <a:ext cx="1102320" cy="911880"/>
+          <a:off x="799920" y="123840"/>
+          <a:ext cx="1092600" cy="911520"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -1786,23 +1732,23 @@
   </sheetPr>
   <dimension ref="1:128"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="false" showRowColHeaders="true" showZeros="false" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A7" colorId="64" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D16" activeCellId="0" sqref="D16"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="false" showRowColHeaders="true" showZeros="false" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A37" colorId="64" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="C68" activeCellId="0" sqref="C68"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.2"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="11.2040816326531"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="7.83163265306122"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="1" width="10.530612244898"/>
-    <col collapsed="false" hidden="false" max="8" min="4" style="1" width="15.5255102040816"/>
-    <col collapsed="false" hidden="false" max="9" min="9" style="1" width="10.530612244898"/>
-    <col collapsed="false" hidden="false" max="10" min="10" style="1" width="18.4948979591837"/>
-    <col collapsed="false" hidden="false" max="12" min="11" style="1" width="8.50510204081633"/>
-    <col collapsed="false" hidden="false" max="13" min="13" style="1" width="1.62244897959184"/>
-    <col collapsed="false" hidden="false" max="14" min="14" style="1" width="9.04591836734694"/>
-    <col collapsed="false" hidden="false" max="15" min="15" style="1" width="10.530612244898"/>
-    <col collapsed="false" hidden="false" max="1025" min="16" style="1" width="9.04591836734694"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="10.9336734693878"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="7.69387755102041"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="1" width="10.3928571428571"/>
+    <col collapsed="false" hidden="false" max="8" min="4" style="1" width="15.3877551020408"/>
+    <col collapsed="false" hidden="false" max="9" min="9" style="1" width="10.3928571428571"/>
+    <col collapsed="false" hidden="false" max="10" min="10" style="1" width="18.2244897959184"/>
+    <col collapsed="false" hidden="false" max="12" min="11" style="1" width="8.36734693877551"/>
+    <col collapsed="false" hidden="false" max="13" min="13" style="1" width="1.48469387755102"/>
+    <col collapsed="false" hidden="false" max="14" min="14" style="1" width="8.77551020408163"/>
+    <col collapsed="false" hidden="false" max="15" min="15" style="1" width="10.3928571428571"/>
+    <col collapsed="false" hidden="false" max="1025" min="16" style="1" width="8.77551020408163"/>
   </cols>
   <sheetData>
     <row r="1" s="2" customFormat="true" ht="20.3" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -17303,7 +17249,6 @@
       <c r="M19" s="28"/>
       <c r="N19" s="0"/>
       <c r="O19" s="0"/>
-      <c r="P19" s="40"/>
       <c r="Q19" s="0"/>
       <c r="R19" s="0"/>
       <c r="S19" s="0"/>
@@ -18336,8 +18281,6 @@
       <c r="K20" s="37"/>
       <c r="L20" s="38"/>
       <c r="M20" s="28"/>
-      <c r="N20" s="40"/>
-      <c r="O20" s="40"/>
       <c r="P20" s="0"/>
       <c r="Q20" s="0"/>
       <c r="R20" s="0"/>
@@ -20376,10 +20319,10 @@
     </row>
     <row r="22" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A22" s="0"/>
-      <c r="B22" s="41"/>
-      <c r="C22" s="41"/>
-      <c r="D22" s="41"/>
-      <c r="E22" s="41"/>
+      <c r="B22" s="28"/>
+      <c r="C22" s="28"/>
+      <c r="D22" s="28"/>
+      <c r="E22" s="28"/>
       <c r="F22" s="0"/>
       <c r="G22" s="0"/>
       <c r="H22" s="0"/>
@@ -22430,27 +22373,27 @@
     </row>
     <row r="24" customFormat="false" ht="17.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A24" s="0"/>
-      <c r="B24" s="42" t="s">
+      <c r="B24" s="40" t="s">
         <v>22</v>
       </c>
-      <c r="C24" s="42"/>
-      <c r="D24" s="42"/>
-      <c r="E24" s="42" t="s">
+      <c r="C24" s="40"/>
+      <c r="D24" s="40"/>
+      <c r="E24" s="40" t="s">
         <v>23</v>
       </c>
-      <c r="F24" s="42" t="s">
+      <c r="F24" s="40" t="s">
         <v>24</v>
       </c>
-      <c r="G24" s="42"/>
-      <c r="H24" s="42" t="s">
+      <c r="G24" s="40"/>
+      <c r="H24" s="40" t="s">
         <v>25</v>
       </c>
-      <c r="I24" s="42"/>
-      <c r="J24" s="42" t="s">
+      <c r="I24" s="40"/>
+      <c r="J24" s="40" t="s">
         <v>26</v>
       </c>
-      <c r="K24" s="42"/>
-      <c r="L24" s="42"/>
+      <c r="K24" s="40"/>
+      <c r="L24" s="40"/>
       <c r="M24" s="0"/>
       <c r="N24" s="0"/>
       <c r="O24" s="0"/>
@@ -23466,25 +23409,25 @@
     </row>
     <row r="25" customFormat="false" ht="13.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A25" s="0"/>
-      <c r="B25" s="43" t="s">
+      <c r="B25" s="41" t="s">
         <v>27</v>
       </c>
-      <c r="C25" s="43"/>
-      <c r="D25" s="43"/>
-      <c r="E25" s="43" t="n">
+      <c r="C25" s="41"/>
+      <c r="D25" s="41"/>
+      <c r="E25" s="41" t="n">
         <v>10</v>
       </c>
-      <c r="F25" s="44" t="s">
+      <c r="F25" s="42" t="s">
         <v>28</v>
       </c>
-      <c r="G25" s="44"/>
-      <c r="H25" s="44" t="s">
+      <c r="G25" s="42"/>
+      <c r="H25" s="42" t="s">
         <v>29</v>
       </c>
-      <c r="I25" s="44"/>
-      <c r="J25" s="43"/>
-      <c r="K25" s="43"/>
-      <c r="L25" s="43"/>
+      <c r="I25" s="42"/>
+      <c r="J25" s="41"/>
+      <c r="K25" s="41"/>
+      <c r="L25" s="41"/>
       <c r="M25" s="0"/>
       <c r="N25" s="0"/>
       <c r="O25" s="0"/>
@@ -24500,17 +24443,17 @@
     </row>
     <row r="26" customFormat="false" ht="18" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A26" s="0"/>
-      <c r="B26" s="45"/>
-      <c r="C26" s="45"/>
-      <c r="D26" s="45"/>
-      <c r="E26" s="45"/>
-      <c r="F26" s="45"/>
-      <c r="G26" s="45"/>
-      <c r="H26" s="46"/>
-      <c r="I26" s="46"/>
-      <c r="J26" s="45"/>
-      <c r="K26" s="45"/>
-      <c r="L26" s="45"/>
+      <c r="B26" s="43"/>
+      <c r="C26" s="43"/>
+      <c r="D26" s="43"/>
+      <c r="E26" s="43"/>
+      <c r="F26" s="43"/>
+      <c r="G26" s="43"/>
+      <c r="H26" s="44"/>
+      <c r="I26" s="44"/>
+      <c r="J26" s="43"/>
+      <c r="K26" s="43"/>
+      <c r="L26" s="43"/>
       <c r="M26" s="0"/>
       <c r="N26" s="0"/>
       <c r="O26" s="0"/>
@@ -26554,35 +26497,35 @@
     </row>
     <row r="28" customFormat="false" ht="32.05" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A28" s="0"/>
-      <c r="B28" s="42" t="s">
+      <c r="B28" s="40" t="s">
         <v>31</v>
       </c>
-      <c r="C28" s="47" t="s">
+      <c r="C28" s="45" t="s">
         <v>32</v>
       </c>
-      <c r="D28" s="47" t="s">
+      <c r="D28" s="45" t="s">
         <v>33</v>
       </c>
-      <c r="E28" s="47" t="s">
+      <c r="E28" s="45" t="s">
         <v>34</v>
       </c>
-      <c r="F28" s="47" t="s">
+      <c r="F28" s="45" t="s">
         <v>35</v>
       </c>
-      <c r="G28" s="47" t="s">
+      <c r="G28" s="45" t="s">
         <v>36</v>
       </c>
-      <c r="H28" s="47" t="s">
+      <c r="H28" s="45" t="s">
         <v>37</v>
       </c>
-      <c r="I28" s="47" t="s">
+      <c r="I28" s="45" t="s">
         <v>38</v>
       </c>
-      <c r="J28" s="42" t="s">
+      <c r="J28" s="40" t="s">
         <v>39</v>
       </c>
-      <c r="K28" s="42"/>
-      <c r="L28" s="42"/>
+      <c r="K28" s="40"/>
+      <c r="L28" s="40"/>
       <c r="M28" s="0"/>
       <c r="N28" s="0"/>
       <c r="O28" s="0"/>
@@ -27598,33 +27541,33 @@
     </row>
     <row r="29" customFormat="false" ht="13.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A29" s="0"/>
-      <c r="B29" s="48" t="s">
+      <c r="B29" s="46" t="s">
         <v>40</v>
       </c>
-      <c r="C29" s="43" t="n">
+      <c r="C29" s="41" t="n">
         <v>2</v>
       </c>
-      <c r="D29" s="48" t="n">
+      <c r="D29" s="46" t="n">
         <v>15</v>
       </c>
-      <c r="E29" s="48" t="s">
+      <c r="E29" s="46" t="s">
         <v>41</v>
       </c>
-      <c r="F29" s="43" t="s">
+      <c r="F29" s="41" t="s">
         <v>42</v>
       </c>
-      <c r="G29" s="48" t="s">
+      <c r="G29" s="46" t="s">
         <v>43</v>
       </c>
-      <c r="H29" s="48" t="s">
+      <c r="H29" s="46" t="s">
         <v>44</v>
       </c>
-      <c r="I29" s="48" t="s">
+      <c r="I29" s="46" t="s">
         <v>45</v>
       </c>
-      <c r="J29" s="48"/>
-      <c r="K29" s="48"/>
-      <c r="L29" s="48"/>
+      <c r="J29" s="46"/>
+      <c r="K29" s="46"/>
+      <c r="L29" s="46"/>
       <c r="M29" s="0"/>
       <c r="N29" s="0"/>
       <c r="O29" s="0"/>
@@ -30694,29 +30637,29 @@
     </row>
     <row r="32" customFormat="false" ht="29.05" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A32" s="0"/>
-      <c r="B32" s="42" t="s">
+      <c r="B32" s="40" t="s">
         <v>47</v>
       </c>
-      <c r="C32" s="42"/>
-      <c r="D32" s="47" t="s">
+      <c r="C32" s="40"/>
+      <c r="D32" s="45" t="s">
         <v>48</v>
       </c>
-      <c r="E32" s="47" t="s">
+      <c r="E32" s="45" t="s">
         <v>49</v>
       </c>
-      <c r="F32" s="47" t="s">
+      <c r="F32" s="45" t="s">
         <v>50</v>
       </c>
-      <c r="G32" s="47"/>
-      <c r="H32" s="47" t="s">
+      <c r="G32" s="45"/>
+      <c r="H32" s="45" t="s">
         <v>51</v>
       </c>
-      <c r="I32" s="47"/>
-      <c r="J32" s="42" t="s">
+      <c r="I32" s="45"/>
+      <c r="J32" s="40" t="s">
         <v>26</v>
       </c>
-      <c r="K32" s="42"/>
-      <c r="L32" s="42"/>
+      <c r="K32" s="40"/>
+      <c r="L32" s="40"/>
       <c r="M32" s="0"/>
       <c r="N32" s="0"/>
       <c r="O32" s="0"/>
@@ -31732,30 +31675,30 @@
     </row>
     <row r="33" customFormat="false" ht="16.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A33" s="0"/>
-      <c r="B33" s="49" t="n">
+      <c r="B33" s="47" t="n">
         <v>72</v>
       </c>
-      <c r="C33" s="49"/>
-      <c r="D33" s="49" t="n">
+      <c r="C33" s="47"/>
+      <c r="D33" s="47" t="n">
         <v>252</v>
       </c>
-      <c r="E33" s="49" t="n">
+      <c r="E33" s="47" t="n">
         <v>0</v>
       </c>
-      <c r="F33" s="49" t="n">
+      <c r="F33" s="47" t="n">
         <f aca="false">SUMIF(J40:J150,"No-Lead Pad",K40:M150)</f>
         <v>0</v>
       </c>
-      <c r="G33" s="49"/>
-      <c r="H33" s="50" t="s">
+      <c r="G33" s="47"/>
+      <c r="H33" s="48" t="s">
         <v>52</v>
       </c>
-      <c r="I33" s="50"/>
-      <c r="J33" s="50" t="s">
+      <c r="I33" s="48"/>
+      <c r="J33" s="48" t="s">
         <v>53</v>
       </c>
-      <c r="K33" s="50"/>
-      <c r="L33" s="50"/>
+      <c r="K33" s="48"/>
+      <c r="L33" s="48"/>
       <c r="M33" s="0"/>
       <c r="N33" s="0"/>
       <c r="O33" s="0"/>
@@ -32771,17 +32714,17 @@
     </row>
     <row r="34" customFormat="false" ht="18" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A34" s="0"/>
-      <c r="B34" s="51"/>
-      <c r="C34" s="52"/>
-      <c r="D34" s="52"/>
-      <c r="E34" s="52"/>
-      <c r="F34" s="52"/>
-      <c r="G34" s="52"/>
-      <c r="H34" s="52"/>
-      <c r="I34" s="52"/>
-      <c r="J34" s="52"/>
-      <c r="K34" s="52"/>
-      <c r="L34" s="52"/>
+      <c r="B34" s="49"/>
+      <c r="C34" s="49"/>
+      <c r="D34" s="49"/>
+      <c r="E34" s="49"/>
+      <c r="F34" s="49"/>
+      <c r="G34" s="49"/>
+      <c r="H34" s="49"/>
+      <c r="I34" s="49"/>
+      <c r="J34" s="49"/>
+      <c r="K34" s="49"/>
+      <c r="L34" s="49"/>
       <c r="M34" s="0"/>
       <c r="N34" s="0"/>
       <c r="O34" s="0"/>
@@ -34825,18 +34768,18 @@
     </row>
     <row r="36" customFormat="false" ht="4.55" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A36" s="0"/>
-      <c r="B36" s="53"/>
-      <c r="C36" s="51"/>
-      <c r="D36" s="51"/>
-      <c r="E36" s="51"/>
-      <c r="F36" s="51"/>
-      <c r="G36" s="51"/>
-      <c r="H36" s="54"/>
-      <c r="I36" s="54"/>
-      <c r="J36" s="54"/>
-      <c r="K36" s="55"/>
-      <c r="L36" s="55"/>
-      <c r="M36" s="56"/>
+      <c r="B36" s="50"/>
+      <c r="C36" s="49"/>
+      <c r="D36" s="49"/>
+      <c r="E36" s="49"/>
+      <c r="F36" s="49"/>
+      <c r="G36" s="49"/>
+      <c r="H36" s="51"/>
+      <c r="I36" s="51"/>
+      <c r="J36" s="51"/>
+      <c r="K36" s="52"/>
+      <c r="L36" s="52"/>
+      <c r="M36" s="53"/>
       <c r="N36" s="0"/>
       <c r="O36" s="0"/>
       <c r="P36" s="0"/>
@@ -35849,38 +35792,38 @@
       <c r="AMI36" s="0"/>
       <c r="AMJ36" s="0"/>
     </row>
-    <row r="37" s="57" customFormat="true" ht="10.2" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B37" s="58" t="s">
+    <row r="37" s="54" customFormat="true" ht="10.2" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="B37" s="55" t="s">
         <v>55</v>
       </c>
-      <c r="C37" s="59"/>
-      <c r="D37" s="59"/>
-      <c r="E37" s="59"/>
-      <c r="F37" s="59"/>
-      <c r="G37" s="59"/>
-      <c r="H37" s="59"/>
-      <c r="I37" s="59"/>
-      <c r="J37" s="59"/>
-      <c r="K37" s="59"/>
-      <c r="L37" s="59"/>
-      <c r="M37" s="60"/>
+      <c r="C37" s="56"/>
+      <c r="D37" s="56"/>
+      <c r="E37" s="56"/>
+      <c r="F37" s="56"/>
+      <c r="G37" s="56"/>
+      <c r="H37" s="56"/>
+      <c r="I37" s="56"/>
+      <c r="J37" s="56"/>
+      <c r="K37" s="56"/>
+      <c r="L37" s="56"/>
+      <c r="M37" s="57"/>
     </row>
     <row r="38" customFormat="false" ht="10.2" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A38" s="57"/>
-      <c r="B38" s="61" t="s">
+      <c r="A38" s="54"/>
+      <c r="B38" s="58" t="s">
         <v>56</v>
       </c>
-      <c r="C38" s="59"/>
-      <c r="D38" s="59"/>
-      <c r="E38" s="59"/>
-      <c r="F38" s="59"/>
-      <c r="G38" s="59"/>
-      <c r="H38" s="59"/>
-      <c r="I38" s="59"/>
-      <c r="J38" s="59"/>
-      <c r="K38" s="59"/>
-      <c r="L38" s="59"/>
-      <c r="M38" s="60"/>
+      <c r="C38" s="56"/>
+      <c r="D38" s="56"/>
+      <c r="E38" s="56"/>
+      <c r="F38" s="56"/>
+      <c r="G38" s="56"/>
+      <c r="H38" s="56"/>
+      <c r="I38" s="56"/>
+      <c r="J38" s="56"/>
+      <c r="K38" s="56"/>
+      <c r="L38" s="56"/>
+      <c r="M38" s="57"/>
       <c r="N38" s="0"/>
       <c r="O38" s="0"/>
       <c r="P38" s="0"/>
@@ -36895,37 +36838,37 @@
     </row>
     <row r="39" customFormat="false" ht="21.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A39" s="0"/>
-      <c r="B39" s="62" t="s">
+      <c r="B39" s="59" t="s">
         <v>57</v>
       </c>
-      <c r="C39" s="62" t="s">
+      <c r="C39" s="59" t="s">
         <v>58</v>
       </c>
-      <c r="D39" s="62" t="s">
+      <c r="D39" s="59" t="s">
         <v>59</v>
       </c>
-      <c r="E39" s="62" t="s">
+      <c r="E39" s="59" t="s">
         <v>60</v>
       </c>
-      <c r="F39" s="62" t="s">
+      <c r="F39" s="59" t="s">
         <v>61</v>
       </c>
-      <c r="G39" s="62" t="s">
+      <c r="G39" s="59" t="s">
         <v>62</v>
       </c>
-      <c r="H39" s="62" t="s">
+      <c r="H39" s="59" t="s">
         <v>63</v>
       </c>
-      <c r="I39" s="62" t="s">
+      <c r="I39" s="59" t="s">
         <v>64</v>
       </c>
-      <c r="J39" s="62" t="s">
+      <c r="J39" s="59" t="s">
         <v>65</v>
       </c>
-      <c r="K39" s="63" t="s">
+      <c r="K39" s="60" t="s">
         <v>66</v>
       </c>
-      <c r="L39" s="63" t="s">
+      <c r="L39" s="60" t="s">
         <v>67</v>
       </c>
       <c r="M39" s="0"/>
@@ -37941,2324 +37884,2324 @@
       <c r="AMI39" s="0"/>
       <c r="AMJ39" s="0"/>
     </row>
-    <row r="40" s="64" customFormat="true" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B40" s="65" t="n">
+    <row r="40" s="61" customFormat="true" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="B40" s="62" t="n">
         <v>1</v>
       </c>
-      <c r="C40" s="66" t="s">
+      <c r="C40" s="63" t="s">
         <v>68</v>
       </c>
-      <c r="D40" s="66" t="s">
+      <c r="D40" s="63" t="s">
         <v>69</v>
       </c>
-      <c r="E40" s="66" t="s">
+      <c r="E40" s="63" t="s">
         <v>70</v>
       </c>
-      <c r="F40" s="66"/>
-      <c r="G40" s="67" t="s">
+      <c r="F40" s="63"/>
+      <c r="G40" s="64" t="s">
         <v>71</v>
       </c>
-      <c r="H40" s="66" t="s">
+      <c r="H40" s="63" t="s">
         <v>70</v>
       </c>
-      <c r="I40" s="66" t="s">
+      <c r="I40" s="63" t="s">
         <v>72</v>
       </c>
-      <c r="J40" s="66" t="s">
+      <c r="J40" s="63" t="s">
         <v>73</v>
       </c>
-      <c r="K40" s="66" t="n">
+      <c r="K40" s="63" t="n">
         <v>1</v>
       </c>
-      <c r="L40" s="68" t="n">
+      <c r="L40" s="65" t="n">
         <f aca="false">K40*$D$25</f>
         <v>0</v>
       </c>
     </row>
-    <row r="41" s="64" customFormat="true" ht="40.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B41" s="65" t="n">
+    <row r="41" s="61" customFormat="true" ht="40.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B41" s="62" t="n">
         <v>2</v>
       </c>
-      <c r="C41" s="66" t="s">
+      <c r="C41" s="63" t="s">
         <v>74</v>
       </c>
-      <c r="D41" s="66" t="s">
+      <c r="D41" s="63" t="s">
         <v>75</v>
       </c>
-      <c r="E41" s="66" t="s">
+      <c r="E41" s="63" t="s">
         <v>76</v>
       </c>
-      <c r="F41" s="66"/>
-      <c r="G41" s="67" t="s">
+      <c r="F41" s="63"/>
+      <c r="G41" s="64" t="s">
         <v>71</v>
       </c>
-      <c r="H41" s="66" t="s">
+      <c r="H41" s="63" t="s">
         <v>76</v>
       </c>
-      <c r="I41" s="66" t="s">
+      <c r="I41" s="63" t="s">
         <v>77</v>
       </c>
-      <c r="J41" s="66" t="s">
+      <c r="J41" s="63" t="s">
         <v>73</v>
       </c>
-      <c r="K41" s="66" t="n">
+      <c r="K41" s="63" t="n">
         <v>2</v>
       </c>
-      <c r="L41" s="68" t="n">
+      <c r="L41" s="65" t="n">
         <f aca="false">K41*$D$25</f>
         <v>0</v>
       </c>
     </row>
     <row r="42" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A42" s="64"/>
-      <c r="B42" s="65" t="n">
+      <c r="A42" s="61"/>
+      <c r="B42" s="62" t="n">
         <v>4</v>
       </c>
-      <c r="C42" s="66" t="s">
+      <c r="C42" s="63" t="s">
         <v>78</v>
       </c>
-      <c r="D42" s="66" t="s">
+      <c r="D42" s="63" t="s">
         <v>79</v>
       </c>
-      <c r="E42" s="66" t="s">
+      <c r="E42" s="63" t="s">
         <v>80</v>
       </c>
-      <c r="F42" s="66"/>
-      <c r="G42" s="67" t="s">
+      <c r="F42" s="63"/>
+      <c r="G42" s="64" t="s">
         <v>71</v>
       </c>
-      <c r="H42" s="66" t="s">
+      <c r="H42" s="63" t="s">
         <v>80</v>
       </c>
-      <c r="I42" s="66" t="s">
+      <c r="I42" s="63" t="s">
         <v>81</v>
       </c>
-      <c r="J42" s="66" t="s">
+      <c r="J42" s="63" t="s">
         <v>73</v>
       </c>
-      <c r="K42" s="66" t="n">
+      <c r="K42" s="63" t="n">
         <v>3</v>
       </c>
-      <c r="L42" s="68" t="n">
+      <c r="L42" s="65" t="n">
         <f aca="false">K42*$D$25</f>
         <v>0</v>
       </c>
     </row>
     <row r="43" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A43" s="64"/>
-      <c r="B43" s="65" t="n">
+      <c r="A43" s="61"/>
+      <c r="B43" s="62" t="n">
         <v>5</v>
       </c>
-      <c r="C43" s="66" t="s">
+      <c r="C43" s="63" t="s">
         <v>82</v>
       </c>
-      <c r="D43" s="66" t="s">
+      <c r="D43" s="63" t="s">
         <v>83</v>
       </c>
-      <c r="E43" s="66" t="s">
+      <c r="E43" s="63" t="s">
         <v>84</v>
       </c>
-      <c r="F43" s="66"/>
-      <c r="G43" s="67" t="s">
+      <c r="F43" s="63"/>
+      <c r="G43" s="64" t="s">
         <v>71</v>
       </c>
-      <c r="H43" s="66" t="s">
+      <c r="H43" s="63" t="s">
         <v>84</v>
       </c>
-      <c r="I43" s="66" t="s">
+      <c r="I43" s="63" t="s">
         <v>85</v>
       </c>
-      <c r="J43" s="66" t="s">
+      <c r="J43" s="63" t="s">
         <v>73</v>
       </c>
-      <c r="K43" s="66" t="n">
+      <c r="K43" s="63" t="n">
         <v>4</v>
       </c>
-      <c r="L43" s="68" t="n">
+      <c r="L43" s="65" t="n">
         <f aca="false">K43*$D$25</f>
         <v>0</v>
       </c>
     </row>
     <row r="44" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A44" s="64"/>
-      <c r="B44" s="65" t="n">
+      <c r="A44" s="61"/>
+      <c r="B44" s="62" t="n">
         <v>6</v>
       </c>
-      <c r="C44" s="66" t="s">
+      <c r="C44" s="63" t="s">
         <v>86</v>
       </c>
-      <c r="D44" s="66" t="s">
+      <c r="D44" s="63" t="s">
         <v>87</v>
       </c>
-      <c r="E44" s="66" t="s">
+      <c r="E44" s="63" t="s">
         <v>88</v>
       </c>
-      <c r="F44" s="66"/>
-      <c r="G44" s="67" t="s">
+      <c r="F44" s="63"/>
+      <c r="G44" s="64" t="s">
         <v>71</v>
       </c>
-      <c r="H44" s="66" t="s">
+      <c r="H44" s="63" t="s">
         <v>88</v>
       </c>
-      <c r="I44" s="66" t="s">
+      <c r="I44" s="63" t="s">
         <v>89</v>
       </c>
-      <c r="J44" s="66" t="s">
+      <c r="J44" s="63" t="s">
         <v>73</v>
       </c>
-      <c r="K44" s="66" t="n">
+      <c r="K44" s="63" t="n">
         <v>2</v>
       </c>
-      <c r="L44" s="68" t="n">
+      <c r="L44" s="65" t="n">
         <f aca="false">K44*$D$25</f>
         <v>0</v>
       </c>
     </row>
     <row r="45" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A45" s="64"/>
-      <c r="B45" s="65" t="n">
+      <c r="A45" s="61"/>
+      <c r="B45" s="62" t="n">
         <v>9</v>
       </c>
-      <c r="C45" s="66" t="s">
+      <c r="C45" s="63" t="s">
         <v>90</v>
       </c>
-      <c r="D45" s="66" t="s">
+      <c r="D45" s="63" t="s">
         <v>91</v>
       </c>
-      <c r="E45" s="66" t="s">
+      <c r="E45" s="63" t="s">
         <v>92</v>
       </c>
-      <c r="F45" s="66"/>
-      <c r="G45" s="67" t="s">
+      <c r="F45" s="63"/>
+      <c r="G45" s="64" t="s">
         <v>71</v>
       </c>
-      <c r="H45" s="66" t="s">
+      <c r="H45" s="63" t="s">
         <v>92</v>
       </c>
-      <c r="I45" s="66" t="s">
+      <c r="I45" s="63" t="s">
         <v>93</v>
       </c>
-      <c r="J45" s="66" t="s">
+      <c r="J45" s="63" t="s">
         <v>73</v>
       </c>
-      <c r="K45" s="66" t="n">
+      <c r="K45" s="63" t="n">
         <v>7</v>
       </c>
-      <c r="L45" s="68" t="n">
+      <c r="L45" s="65" t="n">
         <f aca="false">K45*$D$25</f>
         <v>0</v>
       </c>
     </row>
     <row r="46" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A46" s="64"/>
-      <c r="B46" s="65" t="n">
+      <c r="A46" s="61"/>
+      <c r="B46" s="62" t="n">
         <v>11</v>
       </c>
-      <c r="C46" s="66" t="s">
+      <c r="C46" s="63" t="s">
         <v>94</v>
       </c>
-      <c r="D46" s="66" t="s">
+      <c r="D46" s="63" t="s">
         <v>95</v>
       </c>
-      <c r="E46" s="66" t="s">
+      <c r="E46" s="63" t="s">
         <v>96</v>
       </c>
-      <c r="F46" s="66"/>
-      <c r="G46" s="67" t="s">
+      <c r="F46" s="63"/>
+      <c r="G46" s="64" t="s">
         <v>71</v>
       </c>
-      <c r="H46" s="66" t="s">
+      <c r="H46" s="63" t="s">
         <v>96</v>
       </c>
-      <c r="I46" s="66" t="s">
+      <c r="I46" s="63" t="s">
         <v>97</v>
       </c>
-      <c r="J46" s="66" t="s">
+      <c r="J46" s="63" t="s">
         <v>73</v>
       </c>
-      <c r="K46" s="66" t="n">
+      <c r="K46" s="63" t="n">
         <v>1</v>
       </c>
-      <c r="L46" s="68" t="n">
+      <c r="L46" s="65" t="n">
         <f aca="false">K46*$D$25</f>
         <v>0</v>
       </c>
     </row>
     <row r="47" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A47" s="64"/>
-      <c r="B47" s="65" t="n">
+      <c r="A47" s="61"/>
+      <c r="B47" s="62" t="n">
         <v>14</v>
       </c>
-      <c r="C47" s="66" t="s">
+      <c r="C47" s="63" t="s">
         <v>98</v>
       </c>
-      <c r="D47" s="66"/>
-      <c r="E47" s="66" t="s">
+      <c r="D47" s="63"/>
+      <c r="E47" s="63" t="s">
         <v>99</v>
       </c>
-      <c r="F47" s="66"/>
-      <c r="G47" s="67" t="s">
+      <c r="F47" s="63"/>
+      <c r="G47" s="64" t="s">
         <v>100</v>
       </c>
-      <c r="H47" s="66" t="s">
+      <c r="H47" s="63" t="s">
         <v>99</v>
       </c>
-      <c r="I47" s="66" t="s">
+      <c r="I47" s="63" t="s">
         <v>101</v>
       </c>
-      <c r="J47" s="66" t="s">
+      <c r="J47" s="63" t="s">
         <v>73</v>
       </c>
-      <c r="K47" s="66" t="n">
+      <c r="K47" s="63" t="n">
         <v>1</v>
       </c>
-      <c r="L47" s="68" t="n">
+      <c r="L47" s="65" t="n">
         <f aca="false">K47*$D$25</f>
         <v>0</v>
       </c>
     </row>
     <row r="48" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A48" s="64"/>
-      <c r="B48" s="65" t="n">
+      <c r="A48" s="61"/>
+      <c r="B48" s="62" t="n">
         <v>15</v>
       </c>
-      <c r="C48" s="66" t="s">
+      <c r="C48" s="63" t="s">
         <v>102</v>
       </c>
-      <c r="D48" s="66" t="s">
+      <c r="D48" s="63" t="s">
         <v>83</v>
       </c>
-      <c r="E48" s="66" t="s">
+      <c r="E48" s="63" t="s">
         <v>103</v>
       </c>
-      <c r="F48" s="66"/>
-      <c r="G48" s="67" t="s">
+      <c r="F48" s="63"/>
+      <c r="G48" s="64" t="s">
         <v>71</v>
       </c>
-      <c r="H48" s="66" t="s">
+      <c r="H48" s="63" t="s">
         <v>103</v>
       </c>
-      <c r="I48" s="66" t="s">
+      <c r="I48" s="63" t="s">
         <v>85</v>
       </c>
-      <c r="J48" s="66" t="s">
+      <c r="J48" s="63" t="s">
         <v>73</v>
       </c>
-      <c r="K48" s="66" t="n">
+      <c r="K48" s="63" t="n">
         <v>1</v>
       </c>
-      <c r="L48" s="68" t="n">
+      <c r="L48" s="65" t="n">
         <f aca="false">K48*$D$25</f>
         <v>0</v>
       </c>
     </row>
     <row r="49" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A49" s="64"/>
-      <c r="B49" s="65" t="n">
+      <c r="A49" s="61"/>
+      <c r="B49" s="62" t="n">
         <v>16</v>
       </c>
-      <c r="C49" s="66" t="s">
+      <c r="C49" s="63" t="s">
         <v>104</v>
       </c>
-      <c r="D49" s="66" t="s">
+      <c r="D49" s="63" t="s">
         <v>105</v>
       </c>
-      <c r="E49" s="66" t="s">
+      <c r="E49" s="63" t="s">
         <v>106</v>
       </c>
-      <c r="F49" s="66"/>
-      <c r="G49" s="67" t="s">
+      <c r="F49" s="63"/>
+      <c r="G49" s="64" t="s">
         <v>71</v>
       </c>
-      <c r="H49" s="66" t="s">
+      <c r="H49" s="63" t="s">
         <v>106</v>
       </c>
-      <c r="I49" s="66" t="s">
+      <c r="I49" s="63" t="s">
         <v>107</v>
       </c>
-      <c r="J49" s="66" t="s">
+      <c r="J49" s="63" t="s">
         <v>73</v>
       </c>
-      <c r="K49" s="66" t="n">
+      <c r="K49" s="63" t="n">
         <v>3</v>
       </c>
-      <c r="L49" s="68" t="n">
+      <c r="L49" s="65" t="n">
         <f aca="false">K49*$D$25</f>
         <v>0</v>
       </c>
     </row>
     <row r="50" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A50" s="64"/>
-      <c r="B50" s="65" t="n">
+      <c r="A50" s="61"/>
+      <c r="B50" s="62" t="n">
         <v>17</v>
       </c>
-      <c r="C50" s="66" t="s">
+      <c r="C50" s="63" t="s">
         <v>108</v>
       </c>
-      <c r="D50" s="66" t="s">
+      <c r="D50" s="63" t="s">
         <v>109</v>
       </c>
-      <c r="E50" s="66" t="s">
+      <c r="E50" s="63" t="s">
         <v>110</v>
       </c>
-      <c r="F50" s="66"/>
-      <c r="G50" s="67" t="s">
+      <c r="F50" s="63"/>
+      <c r="G50" s="64" t="s">
         <v>71</v>
       </c>
-      <c r="H50" s="66" t="s">
+      <c r="H50" s="63" t="s">
         <v>110</v>
       </c>
-      <c r="I50" s="66" t="s">
+      <c r="I50" s="63" t="s">
         <v>85</v>
       </c>
-      <c r="J50" s="66" t="s">
+      <c r="J50" s="63" t="s">
         <v>73</v>
       </c>
-      <c r="K50" s="66" t="n">
+      <c r="K50" s="63" t="n">
         <v>19</v>
       </c>
-      <c r="L50" s="68" t="n">
+      <c r="L50" s="65" t="n">
         <f aca="false">K50*$D$25</f>
         <v>0</v>
       </c>
     </row>
     <row r="51" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A51" s="64"/>
-      <c r="B51" s="65" t="n">
+      <c r="A51" s="61"/>
+      <c r="B51" s="62" t="n">
         <v>19</v>
       </c>
-      <c r="C51" s="66" t="s">
+      <c r="C51" s="63" t="s">
         <v>111</v>
       </c>
-      <c r="D51" s="66" t="s">
+      <c r="D51" s="63" t="s">
         <v>112</v>
       </c>
-      <c r="E51" s="66" t="s">
+      <c r="E51" s="63" t="s">
         <v>113</v>
       </c>
-      <c r="F51" s="66"/>
-      <c r="G51" s="67" t="s">
+      <c r="F51" s="63"/>
+      <c r="G51" s="64" t="s">
         <v>114</v>
       </c>
-      <c r="H51" s="66" t="s">
+      <c r="H51" s="63" t="s">
         <v>113</v>
       </c>
-      <c r="I51" s="66" t="s">
+      <c r="I51" s="63" t="s">
         <v>115</v>
       </c>
-      <c r="J51" s="66" t="s">
+      <c r="J51" s="63" t="s">
         <v>73</v>
       </c>
-      <c r="K51" s="66" t="n">
+      <c r="K51" s="63" t="n">
         <v>6</v>
       </c>
-      <c r="L51" s="68" t="n">
+      <c r="L51" s="65" t="n">
         <f aca="false">K51*$D$25</f>
         <v>0</v>
       </c>
     </row>
     <row r="52" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A52" s="64"/>
-      <c r="B52" s="65" t="n">
+      <c r="A52" s="61"/>
+      <c r="B52" s="62" t="n">
         <v>20</v>
       </c>
-      <c r="C52" s="66" t="s">
+      <c r="C52" s="63" t="s">
         <v>116</v>
       </c>
-      <c r="D52" s="66" t="s">
+      <c r="D52" s="63" t="s">
         <v>117</v>
       </c>
-      <c r="E52" s="66" t="s">
+      <c r="E52" s="63" t="s">
         <v>118</v>
       </c>
-      <c r="F52" s="66"/>
-      <c r="G52" s="67" t="s">
+      <c r="F52" s="63"/>
+      <c r="G52" s="64" t="s">
         <v>71</v>
       </c>
-      <c r="H52" s="66" t="s">
+      <c r="H52" s="63" t="s">
         <v>118</v>
       </c>
-      <c r="I52" s="66" t="s">
+      <c r="I52" s="63" t="s">
         <v>119</v>
       </c>
-      <c r="J52" s="66" t="s">
+      <c r="J52" s="63" t="s">
         <v>73</v>
       </c>
-      <c r="K52" s="66" t="n">
+      <c r="K52" s="63" t="n">
         <v>2</v>
       </c>
-      <c r="L52" s="68" t="n">
+      <c r="L52" s="65" t="n">
         <f aca="false">K52*$D$25</f>
         <v>0</v>
       </c>
     </row>
     <row r="53" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A53" s="64"/>
-      <c r="B53" s="65" t="n">
+      <c r="A53" s="61"/>
+      <c r="B53" s="62" t="n">
         <v>21</v>
       </c>
-      <c r="C53" s="66" t="s">
+      <c r="C53" s="63" t="s">
         <v>120</v>
       </c>
-      <c r="D53" s="66" t="s">
+      <c r="D53" s="63" t="s">
         <v>121</v>
       </c>
-      <c r="E53" s="66" t="s">
+      <c r="E53" s="63" t="s">
         <v>122</v>
       </c>
-      <c r="F53" s="66"/>
-      <c r="G53" s="67" t="s">
+      <c r="F53" s="63"/>
+      <c r="G53" s="64" t="s">
         <v>71</v>
       </c>
-      <c r="H53" s="66" t="s">
+      <c r="H53" s="63" t="s">
         <v>122</v>
       </c>
-      <c r="I53" s="66" t="s">
+      <c r="I53" s="63" t="s">
         <v>123</v>
       </c>
-      <c r="J53" s="66" t="s">
+      <c r="J53" s="63" t="s">
         <v>73</v>
       </c>
-      <c r="K53" s="66" t="n">
+      <c r="K53" s="63" t="n">
         <v>4</v>
       </c>
-      <c r="L53" s="68" t="n">
+      <c r="L53" s="65" t="n">
         <f aca="false">K53*$D$25</f>
         <v>0</v>
       </c>
     </row>
     <row r="54" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A54" s="64"/>
-      <c r="B54" s="65" t="n">
+      <c r="A54" s="61"/>
+      <c r="B54" s="62" t="n">
         <v>23</v>
       </c>
-      <c r="C54" s="66" t="s">
+      <c r="C54" s="63" t="s">
         <v>124</v>
       </c>
-      <c r="D54" s="66" t="s">
+      <c r="D54" s="63" t="s">
         <v>125</v>
       </c>
-      <c r="E54" s="66" t="s">
+      <c r="E54" s="63" t="s">
         <v>126</v>
       </c>
-      <c r="F54" s="66"/>
-      <c r="G54" s="67" t="s">
+      <c r="F54" s="63"/>
+      <c r="G54" s="64" t="s">
         <v>71</v>
       </c>
-      <c r="H54" s="66" t="s">
+      <c r="H54" s="63" t="s">
         <v>126</v>
       </c>
-      <c r="I54" s="66" t="s">
+      <c r="I54" s="63" t="s">
         <v>127</v>
       </c>
-      <c r="J54" s="66" t="s">
+      <c r="J54" s="63" t="s">
         <v>73</v>
       </c>
-      <c r="K54" s="66" t="n">
+      <c r="K54" s="63" t="n">
         <v>1</v>
       </c>
-      <c r="L54" s="68" t="n">
+      <c r="L54" s="65" t="n">
         <f aca="false">K54*$D$25</f>
         <v>0</v>
       </c>
     </row>
     <row r="55" customFormat="false" ht="30.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A55" s="64"/>
-      <c r="B55" s="65" t="n">
+      <c r="A55" s="61"/>
+      <c r="B55" s="62" t="n">
         <v>24</v>
       </c>
-      <c r="C55" s="66" t="s">
+      <c r="C55" s="63" t="s">
         <v>128</v>
       </c>
-      <c r="D55" s="66" t="s">
+      <c r="D55" s="63" t="s">
         <v>129</v>
       </c>
-      <c r="E55" s="66" t="s">
+      <c r="E55" s="63" t="s">
         <v>130</v>
       </c>
-      <c r="F55" s="66"/>
-      <c r="G55" s="67" t="s">
+      <c r="F55" s="63"/>
+      <c r="G55" s="64" t="s">
         <v>71</v>
       </c>
-      <c r="H55" s="66" t="s">
+      <c r="H55" s="63" t="s">
         <v>130</v>
       </c>
-      <c r="I55" s="66" t="s">
+      <c r="I55" s="63" t="s">
         <v>119</v>
       </c>
-      <c r="J55" s="66" t="s">
+      <c r="J55" s="63" t="s">
         <v>73</v>
       </c>
-      <c r="K55" s="66" t="n">
+      <c r="K55" s="63" t="n">
         <v>6</v>
       </c>
-      <c r="L55" s="68" t="n">
+      <c r="L55" s="65" t="n">
         <f aca="false">K55*$D$25</f>
         <v>0</v>
       </c>
     </row>
     <row r="56" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A56" s="64"/>
-      <c r="B56" s="65" t="n">
+      <c r="A56" s="61"/>
+      <c r="B56" s="62" t="n">
         <v>25</v>
       </c>
-      <c r="C56" s="66" t="s">
+      <c r="C56" s="63" t="s">
         <v>131</v>
       </c>
-      <c r="D56" s="66" t="s">
+      <c r="D56" s="63" t="s">
         <v>129</v>
       </c>
-      <c r="E56" s="66" t="s">
+      <c r="E56" s="63" t="s">
         <v>132</v>
       </c>
-      <c r="F56" s="66"/>
-      <c r="G56" s="67" t="s">
+      <c r="F56" s="63"/>
+      <c r="G56" s="64" t="s">
         <v>71</v>
       </c>
-      <c r="H56" s="66" t="s">
+      <c r="H56" s="63" t="s">
         <v>132</v>
       </c>
-      <c r="I56" s="66" t="s">
+      <c r="I56" s="63" t="s">
         <v>119</v>
       </c>
-      <c r="J56" s="66" t="s">
+      <c r="J56" s="63" t="s">
         <v>73</v>
       </c>
-      <c r="K56" s="66" t="n">
+      <c r="K56" s="63" t="n">
         <v>10</v>
       </c>
-      <c r="L56" s="68" t="n">
+      <c r="L56" s="65" t="n">
         <f aca="false">K56*$D$25</f>
         <v>0</v>
       </c>
     </row>
     <row r="57" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A57" s="64"/>
-      <c r="B57" s="65" t="n">
+      <c r="A57" s="61"/>
+      <c r="B57" s="62" t="n">
         <v>26</v>
       </c>
-      <c r="C57" s="66" t="s">
+      <c r="C57" s="63" t="s">
         <v>133</v>
       </c>
-      <c r="D57" s="66" t="s">
+      <c r="D57" s="63" t="s">
         <v>134</v>
       </c>
-      <c r="E57" s="66" t="s">
+      <c r="E57" s="63" t="s">
         <v>135</v>
       </c>
-      <c r="F57" s="66"/>
-      <c r="G57" s="67" t="s">
+      <c r="F57" s="63"/>
+      <c r="G57" s="64" t="s">
         <v>71</v>
       </c>
-      <c r="H57" s="66" t="s">
+      <c r="H57" s="63" t="s">
         <v>135</v>
       </c>
-      <c r="I57" s="66" t="s">
+      <c r="I57" s="63" t="s">
         <v>136</v>
       </c>
-      <c r="J57" s="66" t="s">
+      <c r="J57" s="63" t="s">
         <v>73</v>
       </c>
-      <c r="K57" s="66" t="n">
+      <c r="K57" s="63" t="n">
         <v>1</v>
       </c>
-      <c r="L57" s="68" t="n">
+      <c r="L57" s="65" t="n">
         <f aca="false">K57*$D$25</f>
         <v>0</v>
       </c>
     </row>
     <row r="58" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A58" s="64"/>
-      <c r="B58" s="65" t="n">
+      <c r="A58" s="61"/>
+      <c r="B58" s="62" t="n">
         <v>27</v>
       </c>
-      <c r="C58" s="66" t="s">
+      <c r="C58" s="63" t="s">
         <v>137</v>
       </c>
-      <c r="D58" s="66" t="s">
+      <c r="D58" s="63" t="s">
         <v>112</v>
       </c>
-      <c r="E58" s="66" t="s">
+      <c r="E58" s="63" t="s">
         <v>138</v>
       </c>
-      <c r="F58" s="66"/>
-      <c r="G58" s="67" t="s">
+      <c r="F58" s="63"/>
+      <c r="G58" s="64" t="s">
         <v>139</v>
       </c>
-      <c r="H58" s="66" t="s">
+      <c r="H58" s="63" t="s">
         <v>138</v>
       </c>
-      <c r="I58" s="66" t="s">
+      <c r="I58" s="63" t="s">
         <v>115</v>
       </c>
-      <c r="J58" s="66" t="s">
+      <c r="J58" s="63" t="s">
         <v>73</v>
       </c>
-      <c r="K58" s="66" t="n">
+      <c r="K58" s="63" t="n">
         <v>12</v>
       </c>
-      <c r="L58" s="68" t="n">
+      <c r="L58" s="65" t="n">
         <f aca="false">K58*$D$25</f>
         <v>0</v>
       </c>
     </row>
     <row r="59" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A59" s="64"/>
-      <c r="B59" s="65" t="n">
+      <c r="A59" s="61"/>
+      <c r="B59" s="62" t="n">
         <v>28</v>
       </c>
-      <c r="C59" s="66" t="s">
+      <c r="C59" s="63" t="s">
         <v>140</v>
       </c>
-      <c r="D59" s="66" t="s">
+      <c r="D59" s="63" t="s">
         <v>112</v>
       </c>
-      <c r="E59" s="66" t="s">
+      <c r="E59" s="63" t="s">
         <v>141</v>
       </c>
-      <c r="F59" s="66"/>
-      <c r="G59" s="67" t="s">
+      <c r="F59" s="63"/>
+      <c r="G59" s="64" t="s">
         <v>142</v>
       </c>
-      <c r="H59" s="66" t="s">
+      <c r="H59" s="63" t="s">
         <v>141</v>
       </c>
-      <c r="I59" s="66" t="s">
+      <c r="I59" s="63" t="s">
         <v>115</v>
       </c>
-      <c r="J59" s="66" t="s">
+      <c r="J59" s="63" t="s">
         <v>73</v>
       </c>
-      <c r="K59" s="66" t="n">
+      <c r="K59" s="63" t="n">
         <v>8</v>
       </c>
-      <c r="L59" s="68" t="n">
+      <c r="L59" s="65" t="n">
         <f aca="false">K59*$D$25</f>
         <v>0</v>
       </c>
     </row>
     <row r="60" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A60" s="64"/>
-      <c r="B60" s="65" t="n">
+      <c r="A60" s="61"/>
+      <c r="B60" s="62" t="n">
         <v>30</v>
       </c>
-      <c r="C60" s="66" t="s">
+      <c r="C60" s="63" t="s">
         <v>143</v>
       </c>
-      <c r="D60" s="66" t="s">
+      <c r="D60" s="63" t="s">
         <v>144</v>
       </c>
-      <c r="E60" s="66" t="s">
+      <c r="E60" s="63" t="s">
         <v>145</v>
       </c>
-      <c r="F60" s="66"/>
-      <c r="G60" s="67" t="s">
+      <c r="F60" s="63"/>
+      <c r="G60" s="64" t="s">
         <v>71</v>
       </c>
-      <c r="H60" s="66" t="s">
+      <c r="H60" s="63" t="s">
         <v>145</v>
       </c>
-      <c r="I60" s="66" t="s">
+      <c r="I60" s="63" t="s">
         <v>146</v>
       </c>
-      <c r="J60" s="66" t="s">
+      <c r="J60" s="63" t="s">
         <v>73</v>
       </c>
-      <c r="K60" s="66" t="n">
+      <c r="K60" s="63" t="n">
         <v>2</v>
       </c>
-      <c r="L60" s="68" t="n">
+      <c r="L60" s="65" t="n">
         <f aca="false">K60*$D$25</f>
         <v>0</v>
       </c>
     </row>
     <row r="61" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A61" s="64"/>
-      <c r="B61" s="65" t="n">
+      <c r="A61" s="61"/>
+      <c r="B61" s="62" t="n">
         <v>31</v>
       </c>
-      <c r="C61" s="66" t="s">
+      <c r="C61" s="63" t="s">
         <v>147</v>
       </c>
-      <c r="D61" s="66" t="s">
+      <c r="D61" s="63" t="s">
         <v>129</v>
       </c>
-      <c r="E61" s="66" t="s">
+      <c r="E61" s="63" t="s">
         <v>148</v>
       </c>
-      <c r="F61" s="66"/>
-      <c r="G61" s="67" t="s">
+      <c r="F61" s="63"/>
+      <c r="G61" s="64" t="s">
         <v>71</v>
       </c>
-      <c r="H61" s="66" t="s">
+      <c r="H61" s="63" t="s">
         <v>148</v>
       </c>
-      <c r="I61" s="66" t="s">
+      <c r="I61" s="63" t="s">
         <v>119</v>
       </c>
-      <c r="J61" s="66" t="s">
+      <c r="J61" s="63" t="s">
         <v>73</v>
       </c>
-      <c r="K61" s="66" t="n">
+      <c r="K61" s="63" t="n">
         <v>20</v>
       </c>
-      <c r="L61" s="68" t="n">
+      <c r="L61" s="65" t="n">
         <f aca="false">K61*$D$25</f>
         <v>0</v>
       </c>
     </row>
     <row r="62" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A62" s="64"/>
-      <c r="B62" s="65" t="n">
+      <c r="A62" s="61"/>
+      <c r="B62" s="62" t="n">
         <v>34</v>
       </c>
-      <c r="C62" s="66" t="s">
+      <c r="C62" s="63" t="s">
         <v>149</v>
       </c>
-      <c r="D62" s="66" t="s">
+      <c r="D62" s="63" t="s">
         <v>150</v>
       </c>
-      <c r="E62" s="66" t="s">
+      <c r="E62" s="63" t="s">
         <v>151</v>
       </c>
-      <c r="F62" s="66"/>
-      <c r="G62" s="67" t="s">
+      <c r="F62" s="63"/>
+      <c r="G62" s="64" t="s">
         <v>71</v>
       </c>
-      <c r="H62" s="66" t="s">
+      <c r="H62" s="63" t="s">
         <v>151</v>
       </c>
-      <c r="I62" s="66" t="s">
+      <c r="I62" s="63" t="s">
         <v>85</v>
       </c>
-      <c r="J62" s="66" t="s">
+      <c r="J62" s="63" t="s">
         <v>73</v>
       </c>
-      <c r="K62" s="66" t="n">
+      <c r="K62" s="63" t="n">
         <v>4</v>
       </c>
-      <c r="L62" s="68" t="n">
+      <c r="L62" s="65" t="n">
         <f aca="false">K62*$D$25</f>
         <v>0</v>
       </c>
     </row>
     <row r="63" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A63" s="64"/>
-      <c r="B63" s="65" t="n">
+      <c r="A63" s="61"/>
+      <c r="B63" s="62" t="n">
         <v>35</v>
       </c>
-      <c r="C63" s="66" t="s">
+      <c r="C63" s="63" t="s">
         <v>152</v>
       </c>
-      <c r="D63" s="66" t="s">
+      <c r="D63" s="63" t="s">
         <v>129</v>
       </c>
-      <c r="E63" s="66" t="s">
+      <c r="E63" s="63" t="s">
         <v>153</v>
       </c>
-      <c r="F63" s="66"/>
-      <c r="G63" s="67" t="s">
+      <c r="F63" s="63"/>
+      <c r="G63" s="64" t="s">
         <v>71</v>
       </c>
-      <c r="H63" s="66" t="s">
+      <c r="H63" s="63" t="s">
         <v>153</v>
       </c>
-      <c r="I63" s="66" t="s">
+      <c r="I63" s="63" t="s">
         <v>93</v>
       </c>
-      <c r="J63" s="66" t="s">
+      <c r="J63" s="63" t="s">
         <v>73</v>
       </c>
-      <c r="K63" s="66" t="n">
+      <c r="K63" s="63" t="n">
         <v>3</v>
       </c>
-      <c r="L63" s="68" t="n">
+      <c r="L63" s="65" t="n">
         <f aca="false">K63*$D$25</f>
         <v>0</v>
       </c>
     </row>
     <row r="64" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A64" s="64"/>
-      <c r="B64" s="65" t="n">
+      <c r="A64" s="61"/>
+      <c r="B64" s="62" t="n">
         <v>36</v>
       </c>
-      <c r="C64" s="66" t="s">
+      <c r="C64" s="63" t="s">
         <v>154</v>
       </c>
-      <c r="D64" s="66" t="s">
+      <c r="D64" s="63" t="s">
         <v>155</v>
       </c>
-      <c r="E64" s="66" t="s">
+      <c r="E64" s="63" t="s">
         <v>156</v>
       </c>
-      <c r="F64" s="66"/>
-      <c r="G64" s="67" t="s">
+      <c r="F64" s="63"/>
+      <c r="G64" s="64" t="s">
         <v>71</v>
       </c>
-      <c r="H64" s="66" t="s">
+      <c r="H64" s="63" t="s">
         <v>156</v>
       </c>
-      <c r="I64" s="66" t="s">
+      <c r="I64" s="63" t="s">
         <v>157</v>
       </c>
-      <c r="J64" s="66" t="s">
+      <c r="J64" s="63" t="s">
         <v>73</v>
       </c>
-      <c r="K64" s="66" t="n">
+      <c r="K64" s="63" t="n">
         <v>3</v>
       </c>
-      <c r="L64" s="68" t="n">
+      <c r="L64" s="65" t="n">
         <f aca="false">K64*$D$25</f>
         <v>0</v>
       </c>
     </row>
     <row r="65" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A65" s="64"/>
-      <c r="B65" s="65" t="n">
+      <c r="A65" s="61"/>
+      <c r="B65" s="62" t="n">
         <v>38</v>
       </c>
-      <c r="C65" s="66" t="s">
+      <c r="C65" s="63" t="s">
         <v>158</v>
       </c>
-      <c r="D65" s="66" t="s">
+      <c r="D65" s="63" t="s">
         <v>159</v>
       </c>
-      <c r="E65" s="66" t="s">
+      <c r="E65" s="63" t="s">
         <v>160</v>
       </c>
-      <c r="F65" s="66"/>
-      <c r="G65" s="67" t="s">
+      <c r="F65" s="63"/>
+      <c r="G65" s="64" t="s">
         <v>71</v>
       </c>
-      <c r="H65" s="66" t="s">
+      <c r="H65" s="63" t="s">
         <v>160</v>
       </c>
-      <c r="I65" s="66" t="s">
+      <c r="I65" s="63" t="s">
         <v>161</v>
       </c>
-      <c r="J65" s="66" t="s">
+      <c r="J65" s="63" t="s">
         <v>73</v>
       </c>
-      <c r="K65" s="66" t="n">
+      <c r="K65" s="63" t="n">
         <v>1</v>
       </c>
-      <c r="L65" s="68" t="n">
+      <c r="L65" s="65" t="n">
         <f aca="false">K65*$D$25</f>
         <v>0</v>
       </c>
     </row>
     <row r="66" customFormat="false" ht="12.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="B66" s="65" t="n">
+      <c r="B66" s="62" t="n">
         <v>39</v>
       </c>
-      <c r="C66" s="66" t="s">
+      <c r="C66" s="63" t="s">
         <v>162</v>
       </c>
-      <c r="D66" s="66" t="s">
+      <c r="D66" s="63" t="s">
         <v>163</v>
       </c>
-      <c r="E66" s="66" t="s">
+      <c r="E66" s="63" t="s">
         <v>164</v>
       </c>
-      <c r="F66" s="66"/>
-      <c r="G66" s="67" t="s">
+      <c r="F66" s="63"/>
+      <c r="G66" s="64" t="s">
         <v>71</v>
       </c>
-      <c r="H66" s="66" t="s">
+      <c r="H66" s="63" t="s">
         <v>164</v>
       </c>
-      <c r="I66" s="66" t="s">
+      <c r="I66" s="63" t="s">
         <v>165</v>
       </c>
-      <c r="J66" s="66" t="s">
+      <c r="J66" s="63" t="s">
         <v>73</v>
       </c>
-      <c r="K66" s="66" t="n">
+      <c r="K66" s="63" t="n">
         <v>2</v>
       </c>
-      <c r="L66" s="68" t="n">
+      <c r="L66" s="65" t="n">
         <f aca="false">K66*$D$25</f>
         <v>0</v>
       </c>
     </row>
     <row r="67" customFormat="false" ht="20.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B67" s="65" t="n">
+      <c r="B67" s="62" t="n">
         <v>43</v>
       </c>
-      <c r="C67" s="66" t="s">
+      <c r="C67" s="63" t="s">
         <v>166</v>
       </c>
-      <c r="D67" s="66" t="s">
+      <c r="D67" s="63" t="s">
         <v>167</v>
       </c>
-      <c r="E67" s="66" t="s">
+      <c r="E67" s="63" t="s">
         <v>168</v>
       </c>
-      <c r="F67" s="66"/>
-      <c r="G67" s="67" t="s">
+      <c r="F67" s="63"/>
+      <c r="G67" s="64" t="s">
         <v>169</v>
       </c>
-      <c r="H67" s="66" t="s">
+      <c r="H67" s="63" t="s">
         <v>168</v>
       </c>
-      <c r="I67" s="66" t="s">
+      <c r="I67" s="63" t="s">
         <v>115</v>
       </c>
-      <c r="J67" s="66" t="s">
+      <c r="J67" s="63" t="s">
         <v>73</v>
       </c>
-      <c r="K67" s="66" t="n">
+      <c r="K67" s="63" t="n">
         <v>3</v>
       </c>
-      <c r="L67" s="68" t="n">
+      <c r="L67" s="65" t="n">
         <f aca="false">K67*$D$25</f>
         <v>0</v>
       </c>
     </row>
     <row r="68" customFormat="false" ht="21.1" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B68" s="65" t="n">
+      <c r="B68" s="62" t="n">
         <v>44</v>
       </c>
-      <c r="C68" s="66" t="s">
+      <c r="C68" s="63" t="s">
         <v>170</v>
       </c>
-      <c r="D68" s="66" t="s">
+      <c r="D68" s="63" t="s">
         <v>171</v>
       </c>
-      <c r="E68" s="66" t="s">
+      <c r="E68" s="63" t="s">
         <v>172</v>
       </c>
-      <c r="F68" s="66"/>
-      <c r="G68" s="67" t="s">
+      <c r="F68" s="63"/>
+      <c r="G68" s="64" t="s">
         <v>71</v>
       </c>
-      <c r="H68" s="66" t="s">
+      <c r="H68" s="63" t="s">
         <v>172</v>
       </c>
-      <c r="I68" s="66" t="s">
+      <c r="I68" s="63" t="s">
         <v>173</v>
       </c>
-      <c r="J68" s="66" t="s">
+      <c r="J68" s="63" t="s">
         <v>73</v>
       </c>
-      <c r="K68" s="66" t="n">
+      <c r="K68" s="63" t="n">
         <v>3</v>
       </c>
-      <c r="L68" s="68" t="n">
+      <c r="L68" s="65" t="n">
         <f aca="false">K68*$D$25</f>
         <v>0</v>
       </c>
     </row>
     <row r="69" customFormat="false" ht="40.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B69" s="65" t="n">
+      <c r="B69" s="62" t="n">
         <v>47</v>
       </c>
-      <c r="C69" s="66" t="s">
+      <c r="C69" s="63" t="s">
         <v>174</v>
       </c>
-      <c r="D69" s="66" t="s">
+      <c r="D69" s="63" t="s">
         <v>175</v>
       </c>
-      <c r="E69" s="66" t="s">
+      <c r="E69" s="63" t="s">
         <v>176</v>
       </c>
-      <c r="F69" s="66"/>
-      <c r="G69" s="67" t="s">
+      <c r="F69" s="63"/>
+      <c r="G69" s="64" t="s">
         <v>177</v>
       </c>
-      <c r="H69" s="66"/>
-      <c r="I69" s="66" t="s">
+      <c r="H69" s="63"/>
+      <c r="I69" s="63" t="s">
         <v>178</v>
       </c>
-      <c r="J69" s="66" t="s">
+      <c r="J69" s="63" t="s">
         <v>73</v>
       </c>
-      <c r="K69" s="66" t="n">
+      <c r="K69" s="63" t="n">
         <v>8</v>
       </c>
-      <c r="L69" s="68" t="n">
+      <c r="L69" s="65" t="n">
         <f aca="false">K69*$D$25</f>
         <v>0</v>
       </c>
     </row>
     <row r="70" customFormat="false" ht="21.1" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B70" s="65" t="n">
+      <c r="B70" s="62" t="n">
         <v>48</v>
       </c>
-      <c r="C70" s="66" t="s">
+      <c r="C70" s="63" t="s">
         <v>179</v>
       </c>
-      <c r="D70" s="66" t="s">
+      <c r="D70" s="63" t="s">
         <v>171</v>
       </c>
-      <c r="E70" s="66" t="s">
+      <c r="E70" s="63" t="s">
         <v>180</v>
       </c>
-      <c r="F70" s="66"/>
-      <c r="G70" s="67" t="s">
+      <c r="F70" s="63"/>
+      <c r="G70" s="64" t="s">
         <v>71</v>
       </c>
-      <c r="H70" s="66" t="s">
+      <c r="H70" s="63" t="s">
         <v>180</v>
       </c>
-      <c r="I70" s="66" t="s">
+      <c r="I70" s="63" t="s">
         <v>85</v>
       </c>
-      <c r="J70" s="66" t="s">
+      <c r="J70" s="63" t="s">
         <v>73</v>
       </c>
-      <c r="K70" s="66" t="n">
+      <c r="K70" s="63" t="n">
         <v>2</v>
       </c>
-      <c r="L70" s="68" t="n">
+      <c r="L70" s="65" t="n">
         <f aca="false">K70*$D$25</f>
         <v>0</v>
       </c>
     </row>
     <row r="71" customFormat="false" ht="69.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B71" s="65" t="n">
+      <c r="B71" s="62" t="n">
         <v>49</v>
       </c>
-      <c r="C71" s="66" t="s">
+      <c r="C71" s="63" t="s">
         <v>181</v>
       </c>
-      <c r="D71" s="66" t="s">
+      <c r="D71" s="63" t="s">
         <v>83</v>
       </c>
-      <c r="E71" s="66" t="s">
+      <c r="E71" s="63" t="s">
         <v>182</v>
       </c>
-      <c r="F71" s="66"/>
-      <c r="G71" s="67" t="s">
+      <c r="F71" s="63"/>
+      <c r="G71" s="64" t="s">
         <v>71</v>
       </c>
-      <c r="H71" s="66" t="s">
+      <c r="H71" s="63" t="s">
         <v>182</v>
       </c>
-      <c r="I71" s="66" t="s">
+      <c r="I71" s="63" t="s">
         <v>85</v>
       </c>
-      <c r="J71" s="66" t="s">
+      <c r="J71" s="63" t="s">
         <v>73</v>
       </c>
-      <c r="K71" s="66" t="n">
+      <c r="K71" s="63" t="n">
         <v>19</v>
       </c>
-      <c r="L71" s="68" t="n">
+      <c r="L71" s="65" t="n">
         <f aca="false">K71*$D$25</f>
         <v>0</v>
       </c>
     </row>
     <row r="72" customFormat="false" ht="50.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B72" s="65" t="n">
+      <c r="B72" s="62" t="n">
         <v>50</v>
       </c>
-      <c r="C72" s="66" t="s">
+      <c r="C72" s="63" t="s">
         <v>183</v>
       </c>
-      <c r="D72" s="66" t="s">
+      <c r="D72" s="63" t="s">
         <v>184</v>
       </c>
-      <c r="E72" s="66" t="s">
+      <c r="E72" s="63" t="s">
         <v>185</v>
       </c>
-      <c r="F72" s="66"/>
-      <c r="G72" s="67" t="s">
+      <c r="F72" s="63"/>
+      <c r="G72" s="64" t="s">
         <v>71</v>
       </c>
-      <c r="H72" s="66" t="s">
+      <c r="H72" s="63" t="s">
         <v>185</v>
       </c>
-      <c r="I72" s="66" t="s">
+      <c r="I72" s="63" t="s">
         <v>186</v>
       </c>
-      <c r="J72" s="66" t="s">
+      <c r="J72" s="63" t="s">
         <v>73</v>
       </c>
-      <c r="K72" s="66" t="n">
+      <c r="K72" s="63" t="n">
         <v>1</v>
       </c>
-      <c r="L72" s="68" t="n">
+      <c r="L72" s="65" t="n">
         <f aca="false">K72*$D$25</f>
         <v>0</v>
       </c>
     </row>
     <row r="73" customFormat="false" ht="21.1" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B73" s="65" t="n">
+      <c r="B73" s="62" t="n">
         <v>52</v>
       </c>
-      <c r="C73" s="66" t="s">
+      <c r="C73" s="63" t="s">
         <v>187</v>
       </c>
-      <c r="D73" s="66" t="s">
+      <c r="D73" s="63" t="s">
         <v>129</v>
       </c>
-      <c r="E73" s="66" t="s">
+      <c r="E73" s="63" t="s">
         <v>188</v>
       </c>
-      <c r="F73" s="66"/>
-      <c r="G73" s="67" t="s">
+      <c r="F73" s="63"/>
+      <c r="G73" s="64" t="s">
         <v>71</v>
       </c>
-      <c r="H73" s="66" t="s">
+      <c r="H73" s="63" t="s">
         <v>188</v>
       </c>
-      <c r="I73" s="66" t="s">
+      <c r="I73" s="63" t="s">
         <v>119</v>
       </c>
-      <c r="J73" s="66" t="s">
+      <c r="J73" s="63" t="s">
         <v>73</v>
       </c>
-      <c r="K73" s="66" t="n">
+      <c r="K73" s="63" t="n">
         <v>5</v>
       </c>
-      <c r="L73" s="68" t="n">
+      <c r="L73" s="65" t="n">
         <f aca="false">K73*$D$25</f>
         <v>0</v>
       </c>
     </row>
     <row r="74" customFormat="false" ht="21.1" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B74" s="65" t="n">
+      <c r="B74" s="62" t="n">
         <v>54</v>
       </c>
-      <c r="C74" s="66" t="s">
+      <c r="C74" s="63" t="s">
         <v>189</v>
       </c>
-      <c r="D74" s="66" t="s">
+      <c r="D74" s="63" t="s">
         <v>190</v>
       </c>
-      <c r="E74" s="66" t="s">
+      <c r="E74" s="63" t="s">
         <v>191</v>
       </c>
-      <c r="F74" s="66"/>
-      <c r="G74" s="67" t="s">
+      <c r="F74" s="63"/>
+      <c r="G74" s="64" t="s">
         <v>71</v>
       </c>
-      <c r="H74" s="66" t="s">
+      <c r="H74" s="63" t="s">
         <v>191</v>
       </c>
-      <c r="I74" s="66" t="s">
+      <c r="I74" s="63" t="s">
         <v>192</v>
       </c>
-      <c r="J74" s="66" t="s">
+      <c r="J74" s="63" t="s">
         <v>73</v>
       </c>
-      <c r="K74" s="66" t="n">
+      <c r="K74" s="63" t="n">
         <v>7</v>
       </c>
-      <c r="L74" s="68" t="n">
+      <c r="L74" s="65" t="n">
         <f aca="false">K74*$D$25</f>
         <v>0</v>
       </c>
     </row>
     <row r="75" customFormat="false" ht="30.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B75" s="65" t="n">
+      <c r="B75" s="62" t="n">
         <v>55</v>
       </c>
-      <c r="C75" s="66" t="s">
+      <c r="C75" s="63" t="s">
         <v>193</v>
       </c>
-      <c r="D75" s="66" t="s">
+      <c r="D75" s="63" t="s">
         <v>194</v>
       </c>
-      <c r="E75" s="66" t="s">
+      <c r="E75" s="63" t="s">
         <v>195</v>
       </c>
-      <c r="F75" s="66"/>
-      <c r="G75" s="67" t="s">
+      <c r="F75" s="63"/>
+      <c r="G75" s="64" t="s">
         <v>71</v>
       </c>
-      <c r="H75" s="66" t="s">
+      <c r="H75" s="63" t="s">
         <v>195</v>
       </c>
-      <c r="I75" s="66" t="s">
+      <c r="I75" s="63" t="s">
         <v>196</v>
       </c>
-      <c r="J75" s="66" t="s">
+      <c r="J75" s="63" t="s">
         <v>73</v>
       </c>
-      <c r="K75" s="66" t="n">
+      <c r="K75" s="63" t="n">
         <v>1</v>
       </c>
-      <c r="L75" s="68" t="n">
+      <c r="L75" s="65" t="n">
         <f aca="false">K75*$D$25</f>
         <v>0</v>
       </c>
     </row>
     <row r="76" customFormat="false" ht="30.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B76" s="65" t="n">
+      <c r="B76" s="62" t="n">
         <v>56</v>
       </c>
-      <c r="C76" s="66" t="s">
+      <c r="C76" s="63" t="s">
         <v>197</v>
       </c>
-      <c r="D76" s="66" t="s">
+      <c r="D76" s="63" t="s">
         <v>198</v>
       </c>
-      <c r="E76" s="66" t="s">
+      <c r="E76" s="63" t="s">
         <v>199</v>
       </c>
-      <c r="F76" s="66"/>
-      <c r="G76" s="67" t="s">
+      <c r="F76" s="63"/>
+      <c r="G76" s="64" t="s">
         <v>71</v>
       </c>
-      <c r="H76" s="66" t="s">
+      <c r="H76" s="63" t="s">
         <v>199</v>
       </c>
-      <c r="I76" s="66" t="s">
+      <c r="I76" s="63" t="s">
         <v>200</v>
       </c>
-      <c r="J76" s="66" t="s">
+      <c r="J76" s="63" t="s">
         <v>73</v>
       </c>
-      <c r="K76" s="66" t="n">
+      <c r="K76" s="63" t="n">
         <v>1</v>
       </c>
-      <c r="L76" s="68" t="n">
+      <c r="L76" s="65" t="n">
         <f aca="false">K76*$D$25</f>
         <v>0</v>
       </c>
     </row>
     <row r="77" customFormat="false" ht="89.3" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B77" s="65" t="n">
+      <c r="B77" s="62" t="n">
         <v>57</v>
       </c>
-      <c r="C77" s="66" t="s">
+      <c r="C77" s="63" t="s">
         <v>201</v>
       </c>
-      <c r="D77" s="66" t="s">
+      <c r="D77" s="63" t="s">
         <v>129</v>
       </c>
-      <c r="E77" s="66" t="s">
+      <c r="E77" s="63" t="s">
         <v>202</v>
       </c>
-      <c r="F77" s="66"/>
-      <c r="G77" s="67" t="s">
+      <c r="F77" s="63"/>
+      <c r="G77" s="64" t="s">
         <v>71</v>
       </c>
-      <c r="H77" s="66" t="s">
+      <c r="H77" s="63" t="s">
         <v>202</v>
       </c>
-      <c r="I77" s="66" t="s">
+      <c r="I77" s="63" t="s">
         <v>119</v>
       </c>
-      <c r="J77" s="66" t="s">
+      <c r="J77" s="63" t="s">
         <v>73</v>
       </c>
-      <c r="K77" s="66" t="n">
+      <c r="K77" s="63" t="n">
         <v>23</v>
       </c>
-      <c r="L77" s="68" t="n">
+      <c r="L77" s="65" t="n">
         <f aca="false">K77*$D$25</f>
         <v>0</v>
       </c>
     </row>
     <row r="78" customFormat="false" ht="98.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B78" s="65" t="n">
+      <c r="B78" s="62" t="n">
         <v>58</v>
       </c>
-      <c r="C78" s="66" t="s">
+      <c r="C78" s="63" t="s">
         <v>203</v>
       </c>
-      <c r="D78" s="66" t="s">
+      <c r="D78" s="63" t="s">
         <v>129</v>
       </c>
-      <c r="E78" s="66" t="s">
+      <c r="E78" s="63" t="s">
         <v>148</v>
       </c>
-      <c r="F78" s="66"/>
-      <c r="G78" s="67" t="s">
+      <c r="F78" s="63"/>
+      <c r="G78" s="64" t="s">
         <v>71</v>
       </c>
-      <c r="H78" s="66" t="s">
+      <c r="H78" s="63" t="s">
         <v>148</v>
       </c>
-      <c r="I78" s="66" t="s">
+      <c r="I78" s="63" t="s">
         <v>119</v>
       </c>
-      <c r="J78" s="66" t="s">
+      <c r="J78" s="63" t="s">
         <v>73</v>
       </c>
-      <c r="K78" s="66" t="n">
+      <c r="K78" s="63" t="n">
         <v>27</v>
       </c>
-      <c r="L78" s="68" t="n">
+      <c r="L78" s="65" t="n">
         <f aca="false">K78*$D$25</f>
         <v>0</v>
       </c>
     </row>
     <row r="79" customFormat="false" ht="50.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B79" s="65" t="n">
+      <c r="B79" s="62" t="n">
         <v>59</v>
       </c>
-      <c r="C79" s="66" t="s">
+      <c r="C79" s="63" t="s">
         <v>204</v>
       </c>
-      <c r="D79" s="66" t="s">
+      <c r="D79" s="63" t="s">
         <v>205</v>
       </c>
-      <c r="E79" s="66" t="s">
+      <c r="E79" s="63" t="s">
         <v>206</v>
       </c>
-      <c r="F79" s="66"/>
-      <c r="G79" s="67" t="s">
+      <c r="F79" s="63"/>
+      <c r="G79" s="64" t="s">
         <v>71</v>
       </c>
-      <c r="H79" s="66" t="s">
+      <c r="H79" s="63" t="s">
         <v>206</v>
       </c>
-      <c r="I79" s="66" t="s">
+      <c r="I79" s="63" t="s">
         <v>207</v>
       </c>
-      <c r="J79" s="66" t="s">
+      <c r="J79" s="63" t="s">
         <v>73</v>
       </c>
-      <c r="K79" s="66" t="n">
+      <c r="K79" s="63" t="n">
         <v>2</v>
       </c>
-      <c r="L79" s="68" t="n">
+      <c r="L79" s="65" t="n">
         <f aca="false">K79*$D$25</f>
         <v>0</v>
       </c>
     </row>
     <row r="80" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B80" s="65" t="n">
+      <c r="B80" s="62" t="n">
         <v>60</v>
       </c>
-      <c r="C80" s="66" t="s">
+      <c r="C80" s="63" t="s">
         <v>208</v>
       </c>
-      <c r="D80" s="66" t="s">
+      <c r="D80" s="63" t="s">
         <v>117</v>
       </c>
-      <c r="E80" s="66" t="s">
+      <c r="E80" s="63" t="s">
         <v>209</v>
       </c>
-      <c r="F80" s="66"/>
-      <c r="G80" s="67" t="s">
+      <c r="F80" s="63"/>
+      <c r="G80" s="64" t="s">
         <v>71</v>
       </c>
-      <c r="H80" s="66" t="s">
+      <c r="H80" s="63" t="s">
         <v>209</v>
       </c>
-      <c r="I80" s="66" t="s">
+      <c r="I80" s="63" t="s">
         <v>119</v>
       </c>
-      <c r="J80" s="66" t="s">
+      <c r="J80" s="63" t="s">
         <v>73</v>
       </c>
-      <c r="K80" s="66" t="n">
+      <c r="K80" s="63" t="n">
         <v>1</v>
       </c>
-      <c r="L80" s="68" t="n">
+      <c r="L80" s="65" t="n">
         <f aca="false">K80*$D$25</f>
         <v>0</v>
       </c>
     </row>
     <row r="81" customFormat="false" ht="40.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B81" s="65" t="n">
+      <c r="B81" s="62" t="n">
         <v>61</v>
       </c>
-      <c r="C81" s="66" t="s">
+      <c r="C81" s="63" t="s">
         <v>210</v>
       </c>
-      <c r="D81" s="66" t="s">
+      <c r="D81" s="63" t="s">
         <v>211</v>
       </c>
-      <c r="E81" s="66" t="s">
+      <c r="E81" s="63" t="s">
         <v>212</v>
       </c>
-      <c r="F81" s="66"/>
-      <c r="G81" s="67" t="s">
+      <c r="F81" s="63"/>
+      <c r="G81" s="64" t="s">
         <v>71</v>
       </c>
-      <c r="H81" s="66" t="s">
+      <c r="H81" s="63" t="s">
         <v>212</v>
       </c>
-      <c r="I81" s="66" t="s">
+      <c r="I81" s="63" t="s">
         <v>213</v>
       </c>
-      <c r="J81" s="66" t="s">
+      <c r="J81" s="63" t="s">
         <v>73</v>
       </c>
-      <c r="K81" s="66" t="n">
+      <c r="K81" s="63" t="n">
         <v>1</v>
       </c>
-      <c r="L81" s="68" t="n">
+      <c r="L81" s="65" t="n">
         <f aca="false">K81*$D$25</f>
         <v>0</v>
       </c>
     </row>
     <row r="82" customFormat="false" ht="30.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B82" s="65" t="n">
+      <c r="B82" s="62" t="n">
         <v>62</v>
       </c>
-      <c r="C82" s="66" t="s">
+      <c r="C82" s="63" t="s">
         <v>214</v>
       </c>
-      <c r="D82" s="66" t="s">
+      <c r="D82" s="63" t="s">
         <v>215</v>
       </c>
-      <c r="E82" s="66" t="s">
+      <c r="E82" s="63" t="s">
         <v>216</v>
       </c>
-      <c r="F82" s="66"/>
-      <c r="G82" s="67" t="s">
+      <c r="F82" s="63"/>
+      <c r="G82" s="64" t="s">
         <v>71</v>
       </c>
-      <c r="H82" s="66" t="s">
+      <c r="H82" s="63" t="s">
         <v>216</v>
       </c>
-      <c r="I82" s="66" t="s">
+      <c r="I82" s="63" t="s">
         <v>196</v>
       </c>
-      <c r="J82" s="66" t="s">
+      <c r="J82" s="63" t="s">
         <v>73</v>
       </c>
-      <c r="K82" s="66" t="n">
+      <c r="K82" s="63" t="n">
         <v>2</v>
       </c>
-      <c r="L82" s="68" t="n">
+      <c r="L82" s="65" t="n">
         <f aca="false">K82*$D$25</f>
         <v>0</v>
       </c>
     </row>
     <row r="83" customFormat="false" ht="40.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B83" s="65" t="n">
+      <c r="B83" s="62" t="n">
         <v>63</v>
       </c>
-      <c r="C83" s="66" t="s">
+      <c r="C83" s="63" t="s">
         <v>217</v>
       </c>
-      <c r="D83" s="66" t="s">
+      <c r="D83" s="63" t="s">
         <v>218</v>
       </c>
-      <c r="E83" s="66" t="s">
+      <c r="E83" s="63" t="s">
         <v>219</v>
       </c>
-      <c r="F83" s="66"/>
-      <c r="G83" s="67" t="s">
+      <c r="F83" s="63"/>
+      <c r="G83" s="64" t="s">
         <v>218</v>
       </c>
-      <c r="H83" s="66" t="s">
+      <c r="H83" s="63" t="s">
         <v>219</v>
       </c>
-      <c r="I83" s="66" t="s">
+      <c r="I83" s="63" t="s">
         <v>220</v>
       </c>
-      <c r="J83" s="66" t="s">
+      <c r="J83" s="63" t="s">
         <v>73</v>
       </c>
-      <c r="K83" s="66" t="n">
+      <c r="K83" s="63" t="n">
         <v>2</v>
       </c>
-      <c r="L83" s="68" t="n">
+      <c r="L83" s="65" t="n">
         <f aca="false">K83*$D$25</f>
         <v>0</v>
       </c>
     </row>
     <row r="84" customFormat="false" ht="21.1" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B84" s="65" t="n">
+      <c r="B84" s="62" t="n">
         <v>64</v>
       </c>
-      <c r="C84" s="66" t="s">
+      <c r="C84" s="63" t="s">
         <v>221</v>
       </c>
-      <c r="D84" s="66" t="s">
+      <c r="D84" s="63" t="s">
         <v>129</v>
       </c>
-      <c r="E84" s="66" t="s">
+      <c r="E84" s="63" t="s">
         <v>222</v>
       </c>
-      <c r="F84" s="66"/>
-      <c r="G84" s="67" t="s">
+      <c r="F84" s="63"/>
+      <c r="G84" s="64" t="s">
         <v>71</v>
       </c>
-      <c r="H84" s="66" t="s">
+      <c r="H84" s="63" t="s">
         <v>222</v>
       </c>
-      <c r="I84" s="66" t="s">
+      <c r="I84" s="63" t="s">
         <v>119</v>
       </c>
-      <c r="J84" s="66" t="s">
+      <c r="J84" s="63" t="s">
         <v>73</v>
       </c>
-      <c r="K84" s="66" t="n">
+      <c r="K84" s="63" t="n">
         <v>3</v>
       </c>
-      <c r="L84" s="68" t="n">
+      <c r="L84" s="65" t="n">
         <f aca="false">K84*$D$25</f>
         <v>0</v>
       </c>
     </row>
     <row r="85" customFormat="false" ht="30.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B85" s="65" t="n">
+      <c r="B85" s="62" t="n">
         <v>67</v>
       </c>
-      <c r="C85" s="66" t="s">
+      <c r="C85" s="63" t="s">
         <v>223</v>
       </c>
-      <c r="D85" s="66" t="s">
+      <c r="D85" s="63" t="s">
         <v>224</v>
       </c>
-      <c r="E85" s="66" t="s">
+      <c r="E85" s="63" t="s">
         <v>225</v>
       </c>
-      <c r="F85" s="66"/>
-      <c r="G85" s="67" t="s">
+      <c r="F85" s="63"/>
+      <c r="G85" s="64" t="s">
         <v>71</v>
       </c>
-      <c r="H85" s="66" t="s">
+      <c r="H85" s="63" t="s">
         <v>225</v>
       </c>
-      <c r="I85" s="66" t="s">
+      <c r="I85" s="63" t="s">
         <v>226</v>
       </c>
-      <c r="J85" s="66" t="s">
+      <c r="J85" s="63" t="s">
         <v>73</v>
       </c>
-      <c r="K85" s="66" t="n">
+      <c r="K85" s="63" t="n">
         <v>2</v>
       </c>
-      <c r="L85" s="68" t="n">
+      <c r="L85" s="65" t="n">
         <f aca="false">K85*$D$25</f>
         <v>0</v>
       </c>
     </row>
     <row r="86" customFormat="false" ht="20.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B86" s="65" t="n">
+      <c r="B86" s="62" t="n">
         <v>68</v>
       </c>
-      <c r="C86" s="66" t="s">
+      <c r="C86" s="63" t="s">
         <v>227</v>
       </c>
-      <c r="D86" s="66" t="s">
+      <c r="D86" s="63" t="s">
         <v>175</v>
       </c>
-      <c r="E86" s="66"/>
-      <c r="F86" s="66"/>
-      <c r="G86" s="67" t="s">
+      <c r="E86" s="63"/>
+      <c r="F86" s="63"/>
+      <c r="G86" s="64" t="s">
         <v>228</v>
       </c>
-      <c r="H86" s="66"/>
-      <c r="I86" s="66" t="s">
+      <c r="H86" s="63"/>
+      <c r="I86" s="63" t="s">
         <v>115</v>
       </c>
-      <c r="J86" s="66" t="s">
+      <c r="J86" s="63" t="s">
         <v>73</v>
       </c>
-      <c r="K86" s="66" t="n">
+      <c r="K86" s="63" t="n">
         <v>4</v>
       </c>
-      <c r="L86" s="68" t="n">
+      <c r="L86" s="65" t="n">
         <f aca="false">K86*$D$25</f>
         <v>0</v>
       </c>
     </row>
     <row r="87" customFormat="false" ht="21.1" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B87" s="65" t="n">
+      <c r="B87" s="62" t="n">
         <v>70</v>
       </c>
-      <c r="C87" s="66" t="s">
+      <c r="C87" s="63" t="s">
         <v>229</v>
       </c>
-      <c r="D87" s="66" t="s">
+      <c r="D87" s="63" t="s">
         <v>83</v>
       </c>
-      <c r="E87" s="66" t="s">
+      <c r="E87" s="63" t="s">
         <v>230</v>
       </c>
-      <c r="F87" s="66"/>
-      <c r="G87" s="67" t="s">
+      <c r="F87" s="63"/>
+      <c r="G87" s="64" t="s">
         <v>71</v>
       </c>
-      <c r="H87" s="66" t="s">
+      <c r="H87" s="63" t="s">
         <v>230</v>
       </c>
-      <c r="I87" s="66" t="s">
+      <c r="I87" s="63" t="s">
         <v>107</v>
       </c>
-      <c r="J87" s="66" t="s">
+      <c r="J87" s="63" t="s">
         <v>73</v>
       </c>
-      <c r="K87" s="66" t="n">
+      <c r="K87" s="63" t="n">
         <v>5</v>
       </c>
-      <c r="L87" s="68" t="n">
+      <c r="L87" s="65" t="n">
         <f aca="false">K87*$D$25</f>
         <v>0</v>
       </c>
     </row>
     <row r="88" customFormat="false" ht="40.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B88" s="65" t="n">
+      <c r="B88" s="62" t="n">
         <v>72</v>
       </c>
-      <c r="C88" s="66" t="s">
+      <c r="C88" s="63" t="s">
         <v>231</v>
       </c>
-      <c r="D88" s="66" t="s">
+      <c r="D88" s="63" t="s">
         <v>232</v>
       </c>
-      <c r="E88" s="66" t="s">
+      <c r="E88" s="63" t="s">
         <v>233</v>
       </c>
-      <c r="F88" s="66"/>
-      <c r="G88" s="67" t="s">
+      <c r="F88" s="63"/>
+      <c r="G88" s="64" t="s">
         <v>71</v>
       </c>
-      <c r="H88" s="66" t="s">
+      <c r="H88" s="63" t="s">
         <v>233</v>
       </c>
-      <c r="I88" s="66" t="s">
+      <c r="I88" s="63" t="s">
         <v>234</v>
       </c>
-      <c r="J88" s="66" t="s">
+      <c r="J88" s="63" t="s">
         <v>73</v>
       </c>
-      <c r="K88" s="66" t="n">
+      <c r="K88" s="63" t="n">
         <v>1</v>
       </c>
-      <c r="L88" s="68" t="n">
+      <c r="L88" s="65" t="n">
         <f aca="false">K88*$D$25</f>
         <v>0</v>
       </c>
     </row>
     <row r="89" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B89" s="65"/>
-      <c r="C89" s="66"/>
-      <c r="D89" s="66"/>
-      <c r="E89" s="66"/>
-      <c r="F89" s="66"/>
-      <c r="G89" s="67"/>
-      <c r="H89" s="66"/>
-      <c r="I89" s="66"/>
-      <c r="J89" s="66"/>
-      <c r="K89" s="66"/>
-      <c r="L89" s="68" t="n">
+      <c r="B89" s="62"/>
+      <c r="C89" s="63"/>
+      <c r="D89" s="63"/>
+      <c r="E89" s="63"/>
+      <c r="F89" s="63"/>
+      <c r="G89" s="64"/>
+      <c r="H89" s="63"/>
+      <c r="I89" s="63"/>
+      <c r="J89" s="63"/>
+      <c r="K89" s="63"/>
+      <c r="L89" s="65" t="n">
         <f aca="false">K89*$D$25</f>
         <v>0</v>
       </c>
     </row>
     <row r="90" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B90" s="65"/>
-      <c r="C90" s="66"/>
-      <c r="D90" s="66"/>
-      <c r="E90" s="66"/>
-      <c r="F90" s="66"/>
-      <c r="G90" s="67"/>
-      <c r="H90" s="66"/>
-      <c r="I90" s="66"/>
-      <c r="J90" s="66"/>
-      <c r="K90" s="66"/>
-      <c r="L90" s="68" t="n">
+      <c r="B90" s="62"/>
+      <c r="C90" s="63"/>
+      <c r="D90" s="63"/>
+      <c r="E90" s="63"/>
+      <c r="F90" s="63"/>
+      <c r="G90" s="64"/>
+      <c r="H90" s="63"/>
+      <c r="I90" s="63"/>
+      <c r="J90" s="63"/>
+      <c r="K90" s="63"/>
+      <c r="L90" s="65" t="n">
         <f aca="false">K90*$D$25</f>
         <v>0</v>
       </c>
     </row>
     <row r="91" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B91" s="65"/>
-      <c r="C91" s="66"/>
-      <c r="D91" s="66"/>
-      <c r="E91" s="66"/>
-      <c r="F91" s="66"/>
-      <c r="G91" s="67"/>
-      <c r="H91" s="66"/>
-      <c r="I91" s="66"/>
-      <c r="J91" s="66"/>
-      <c r="K91" s="66"/>
-      <c r="L91" s="68" t="n">
+      <c r="B91" s="62"/>
+      <c r="C91" s="63"/>
+      <c r="D91" s="63"/>
+      <c r="E91" s="63"/>
+      <c r="F91" s="63"/>
+      <c r="G91" s="64"/>
+      <c r="H91" s="63"/>
+      <c r="I91" s="63"/>
+      <c r="J91" s="63"/>
+      <c r="K91" s="63"/>
+      <c r="L91" s="65" t="n">
         <f aca="false">K91*$D$25</f>
         <v>0</v>
       </c>
     </row>
     <row r="92" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B92" s="65"/>
-      <c r="C92" s="66"/>
-      <c r="D92" s="66"/>
-      <c r="E92" s="66"/>
-      <c r="F92" s="66"/>
-      <c r="G92" s="67"/>
-      <c r="H92" s="66"/>
-      <c r="I92" s="66"/>
-      <c r="J92" s="66"/>
-      <c r="K92" s="66"/>
-      <c r="L92" s="68" t="n">
+      <c r="B92" s="62"/>
+      <c r="C92" s="63"/>
+      <c r="D92" s="63"/>
+      <c r="E92" s="63"/>
+      <c r="F92" s="63"/>
+      <c r="G92" s="64"/>
+      <c r="H92" s="63"/>
+      <c r="I92" s="63"/>
+      <c r="J92" s="63"/>
+      <c r="K92" s="63"/>
+      <c r="L92" s="65" t="n">
         <f aca="false">K92*$D$25</f>
         <v>0</v>
       </c>
     </row>
     <row r="93" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B93" s="65"/>
-      <c r="C93" s="66"/>
-      <c r="D93" s="66"/>
-      <c r="E93" s="66"/>
-      <c r="F93" s="66"/>
-      <c r="G93" s="67"/>
-      <c r="H93" s="66"/>
-      <c r="I93" s="66"/>
-      <c r="J93" s="66"/>
-      <c r="K93" s="66"/>
-      <c r="L93" s="68" t="n">
+      <c r="B93" s="62"/>
+      <c r="C93" s="63"/>
+      <c r="D93" s="63"/>
+      <c r="E93" s="63"/>
+      <c r="F93" s="63"/>
+      <c r="G93" s="64"/>
+      <c r="H93" s="63"/>
+      <c r="I93" s="63"/>
+      <c r="J93" s="63"/>
+      <c r="K93" s="63"/>
+      <c r="L93" s="65" t="n">
         <f aca="false">K93*$D$25</f>
         <v>0</v>
       </c>
     </row>
     <row r="94" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B94" s="65"/>
-      <c r="C94" s="66"/>
-      <c r="D94" s="66"/>
-      <c r="E94" s="66"/>
-      <c r="F94" s="66"/>
-      <c r="G94" s="67"/>
-      <c r="H94" s="66"/>
-      <c r="I94" s="66"/>
-      <c r="J94" s="66"/>
-      <c r="K94" s="66"/>
-      <c r="L94" s="68" t="n">
+      <c r="B94" s="62"/>
+      <c r="C94" s="63"/>
+      <c r="D94" s="63"/>
+      <c r="E94" s="63"/>
+      <c r="F94" s="63"/>
+      <c r="G94" s="64"/>
+      <c r="H94" s="63"/>
+      <c r="I94" s="63"/>
+      <c r="J94" s="63"/>
+      <c r="K94" s="63"/>
+      <c r="L94" s="65" t="n">
         <f aca="false">K94*$D$25</f>
         <v>0</v>
       </c>
     </row>
     <row r="95" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B95" s="65"/>
-      <c r="C95" s="66"/>
-      <c r="D95" s="66"/>
-      <c r="E95" s="66"/>
-      <c r="F95" s="66"/>
-      <c r="G95" s="67"/>
-      <c r="H95" s="66"/>
-      <c r="I95" s="66"/>
-      <c r="J95" s="66"/>
-      <c r="K95" s="66"/>
-      <c r="L95" s="68" t="n">
+      <c r="B95" s="62"/>
+      <c r="C95" s="63"/>
+      <c r="D95" s="63"/>
+      <c r="E95" s="63"/>
+      <c r="F95" s="63"/>
+      <c r="G95" s="64"/>
+      <c r="H95" s="63"/>
+      <c r="I95" s="63"/>
+      <c r="J95" s="63"/>
+      <c r="K95" s="63"/>
+      <c r="L95" s="65" t="n">
         <f aca="false">K95*$D$25</f>
         <v>0</v>
       </c>
     </row>
     <row r="96" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B96" s="65"/>
-      <c r="C96" s="66"/>
-      <c r="D96" s="66"/>
-      <c r="E96" s="66"/>
-      <c r="F96" s="66"/>
-      <c r="G96" s="67"/>
-      <c r="H96" s="66"/>
-      <c r="I96" s="66"/>
-      <c r="J96" s="66"/>
-      <c r="K96" s="66"/>
-      <c r="L96" s="68" t="n">
+      <c r="B96" s="62"/>
+      <c r="C96" s="63"/>
+      <c r="D96" s="63"/>
+      <c r="E96" s="63"/>
+      <c r="F96" s="63"/>
+      <c r="G96" s="64"/>
+      <c r="H96" s="63"/>
+      <c r="I96" s="63"/>
+      <c r="J96" s="63"/>
+      <c r="K96" s="63"/>
+      <c r="L96" s="65" t="n">
         <f aca="false">K96*$D$25</f>
         <v>0</v>
       </c>
     </row>
     <row r="97" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B97" s="65"/>
-      <c r="C97" s="66"/>
-      <c r="D97" s="66"/>
-      <c r="E97" s="66"/>
-      <c r="F97" s="66"/>
-      <c r="G97" s="67"/>
-      <c r="H97" s="66"/>
-      <c r="I97" s="66"/>
-      <c r="J97" s="66"/>
-      <c r="K97" s="66"/>
-      <c r="L97" s="68" t="n">
+      <c r="B97" s="62"/>
+      <c r="C97" s="63"/>
+      <c r="D97" s="63"/>
+      <c r="E97" s="63"/>
+      <c r="F97" s="63"/>
+      <c r="G97" s="64"/>
+      <c r="H97" s="63"/>
+      <c r="I97" s="63"/>
+      <c r="J97" s="63"/>
+      <c r="K97" s="63"/>
+      <c r="L97" s="65" t="n">
         <f aca="false">K97*$D$25</f>
         <v>0</v>
       </c>
     </row>
     <row r="98" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B98" s="65"/>
-      <c r="C98" s="66"/>
-      <c r="D98" s="66"/>
-      <c r="E98" s="66"/>
-      <c r="F98" s="66"/>
-      <c r="G98" s="67"/>
-      <c r="H98" s="66"/>
-      <c r="I98" s="66"/>
-      <c r="J98" s="66"/>
-      <c r="K98" s="66"/>
-      <c r="L98" s="68" t="n">
+      <c r="B98" s="62"/>
+      <c r="C98" s="63"/>
+      <c r="D98" s="63"/>
+      <c r="E98" s="63"/>
+      <c r="F98" s="63"/>
+      <c r="G98" s="64"/>
+      <c r="H98" s="63"/>
+      <c r="I98" s="63"/>
+      <c r="J98" s="63"/>
+      <c r="K98" s="63"/>
+      <c r="L98" s="65" t="n">
         <f aca="false">K98*$D$25</f>
         <v>0</v>
       </c>
     </row>
     <row r="99" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B99" s="65"/>
-      <c r="C99" s="66"/>
-      <c r="D99" s="66"/>
-      <c r="E99" s="66"/>
-      <c r="F99" s="66"/>
-      <c r="G99" s="67"/>
-      <c r="H99" s="66"/>
-      <c r="I99" s="66"/>
-      <c r="J99" s="66"/>
-      <c r="K99" s="66"/>
-      <c r="L99" s="68" t="n">
+      <c r="B99" s="62"/>
+      <c r="C99" s="63"/>
+      <c r="D99" s="63"/>
+      <c r="E99" s="63"/>
+      <c r="F99" s="63"/>
+      <c r="G99" s="64"/>
+      <c r="H99" s="63"/>
+      <c r="I99" s="63"/>
+      <c r="J99" s="63"/>
+      <c r="K99" s="63"/>
+      <c r="L99" s="65" t="n">
         <f aca="false">K99*$D$25</f>
         <v>0</v>
       </c>
     </row>
     <row r="100" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B100" s="65"/>
-      <c r="C100" s="66"/>
-      <c r="D100" s="66"/>
-      <c r="E100" s="66"/>
-      <c r="F100" s="66"/>
-      <c r="G100" s="67"/>
-      <c r="H100" s="66"/>
-      <c r="I100" s="66"/>
-      <c r="J100" s="66"/>
-      <c r="K100" s="66"/>
-      <c r="L100" s="68" t="n">
+      <c r="B100" s="62"/>
+      <c r="C100" s="63"/>
+      <c r="D100" s="63"/>
+      <c r="E100" s="63"/>
+      <c r="F100" s="63"/>
+      <c r="G100" s="64"/>
+      <c r="H100" s="63"/>
+      <c r="I100" s="63"/>
+      <c r="J100" s="63"/>
+      <c r="K100" s="63"/>
+      <c r="L100" s="65" t="n">
         <f aca="false">K100*$D$25</f>
         <v>0</v>
       </c>
     </row>
     <row r="101" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B101" s="65"/>
-      <c r="C101" s="66"/>
-      <c r="D101" s="66"/>
-      <c r="E101" s="66"/>
-      <c r="F101" s="66"/>
-      <c r="G101" s="67"/>
-      <c r="H101" s="66"/>
-      <c r="I101" s="66"/>
-      <c r="J101" s="66"/>
-      <c r="K101" s="66"/>
-      <c r="L101" s="68" t="n">
+      <c r="B101" s="62"/>
+      <c r="C101" s="63"/>
+      <c r="D101" s="63"/>
+      <c r="E101" s="63"/>
+      <c r="F101" s="63"/>
+      <c r="G101" s="64"/>
+      <c r="H101" s="63"/>
+      <c r="I101" s="63"/>
+      <c r="J101" s="63"/>
+      <c r="K101" s="63"/>
+      <c r="L101" s="65" t="n">
         <f aca="false">K101*$D$25</f>
         <v>0</v>
       </c>
     </row>
     <row r="102" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B102" s="65"/>
-      <c r="C102" s="66"/>
-      <c r="D102" s="66"/>
-      <c r="E102" s="66"/>
-      <c r="F102" s="66"/>
-      <c r="G102" s="67"/>
-      <c r="H102" s="66"/>
-      <c r="I102" s="66"/>
-      <c r="J102" s="66"/>
-      <c r="K102" s="66"/>
-      <c r="L102" s="68" t="n">
+      <c r="B102" s="62"/>
+      <c r="C102" s="63"/>
+      <c r="D102" s="63"/>
+      <c r="E102" s="63"/>
+      <c r="F102" s="63"/>
+      <c r="G102" s="64"/>
+      <c r="H102" s="63"/>
+      <c r="I102" s="63"/>
+      <c r="J102" s="63"/>
+      <c r="K102" s="63"/>
+      <c r="L102" s="65" t="n">
         <f aca="false">K102*$D$25</f>
         <v>0</v>
       </c>
     </row>
     <row r="103" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B103" s="65"/>
-      <c r="C103" s="66"/>
-      <c r="D103" s="66"/>
-      <c r="E103" s="66"/>
-      <c r="F103" s="66"/>
-      <c r="G103" s="67"/>
-      <c r="H103" s="66"/>
-      <c r="I103" s="66"/>
-      <c r="J103" s="66"/>
-      <c r="K103" s="66"/>
-      <c r="L103" s="68" t="n">
+      <c r="B103" s="62"/>
+      <c r="C103" s="63"/>
+      <c r="D103" s="63"/>
+      <c r="E103" s="63"/>
+      <c r="F103" s="63"/>
+      <c r="G103" s="64"/>
+      <c r="H103" s="63"/>
+      <c r="I103" s="63"/>
+      <c r="J103" s="63"/>
+      <c r="K103" s="63"/>
+      <c r="L103" s="65" t="n">
         <f aca="false">K103*$D$25</f>
         <v>0</v>
       </c>
     </row>
     <row r="104" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B104" s="65"/>
-      <c r="C104" s="66"/>
-      <c r="D104" s="66"/>
-      <c r="E104" s="66"/>
-      <c r="F104" s="66"/>
-      <c r="G104" s="67"/>
-      <c r="H104" s="66"/>
-      <c r="I104" s="66"/>
-      <c r="J104" s="66"/>
-      <c r="K104" s="66"/>
-      <c r="L104" s="68" t="n">
+      <c r="B104" s="62"/>
+      <c r="C104" s="63"/>
+      <c r="D104" s="63"/>
+      <c r="E104" s="63"/>
+      <c r="F104" s="63"/>
+      <c r="G104" s="64"/>
+      <c r="H104" s="63"/>
+      <c r="I104" s="63"/>
+      <c r="J104" s="63"/>
+      <c r="K104" s="63"/>
+      <c r="L104" s="65" t="n">
         <f aca="false">K104*$D$25</f>
         <v>0</v>
       </c>
     </row>
     <row r="105" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B105" s="65"/>
-      <c r="C105" s="66"/>
-      <c r="D105" s="66"/>
-      <c r="E105" s="66"/>
-      <c r="F105" s="66"/>
-      <c r="G105" s="67"/>
-      <c r="H105" s="66"/>
-      <c r="I105" s="66"/>
-      <c r="J105" s="66"/>
-      <c r="K105" s="66"/>
-      <c r="L105" s="68" t="n">
+      <c r="B105" s="62"/>
+      <c r="C105" s="63"/>
+      <c r="D105" s="63"/>
+      <c r="E105" s="63"/>
+      <c r="F105" s="63"/>
+      <c r="G105" s="64"/>
+      <c r="H105" s="63"/>
+      <c r="I105" s="63"/>
+      <c r="J105" s="63"/>
+      <c r="K105" s="63"/>
+      <c r="L105" s="65" t="n">
         <f aca="false">K105*$D$25</f>
         <v>0</v>
       </c>
     </row>
     <row r="106" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B106" s="65"/>
-      <c r="C106" s="66"/>
-      <c r="D106" s="66"/>
-      <c r="E106" s="66"/>
-      <c r="F106" s="66"/>
-      <c r="G106" s="67"/>
-      <c r="H106" s="66"/>
-      <c r="I106" s="66"/>
-      <c r="J106" s="66"/>
-      <c r="K106" s="66"/>
-      <c r="L106" s="68" t="n">
+      <c r="B106" s="62"/>
+      <c r="C106" s="63"/>
+      <c r="D106" s="63"/>
+      <c r="E106" s="63"/>
+      <c r="F106" s="63"/>
+      <c r="G106" s="64"/>
+      <c r="H106" s="63"/>
+      <c r="I106" s="63"/>
+      <c r="J106" s="63"/>
+      <c r="K106" s="63"/>
+      <c r="L106" s="65" t="n">
         <f aca="false">K106*$D$25</f>
         <v>0</v>
       </c>
     </row>
     <row r="107" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B107" s="65"/>
-      <c r="C107" s="66"/>
-      <c r="D107" s="66"/>
-      <c r="E107" s="66"/>
-      <c r="F107" s="66"/>
-      <c r="G107" s="67"/>
-      <c r="H107" s="66"/>
-      <c r="I107" s="66"/>
-      <c r="J107" s="66"/>
-      <c r="K107" s="66"/>
-      <c r="L107" s="68" t="n">
+      <c r="B107" s="62"/>
+      <c r="C107" s="63"/>
+      <c r="D107" s="63"/>
+      <c r="E107" s="63"/>
+      <c r="F107" s="63"/>
+      <c r="G107" s="64"/>
+      <c r="H107" s="63"/>
+      <c r="I107" s="63"/>
+      <c r="J107" s="63"/>
+      <c r="K107" s="63"/>
+      <c r="L107" s="65" t="n">
         <f aca="false">K107*$D$25</f>
         <v>0</v>
       </c>
     </row>
     <row r="108" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B108" s="65"/>
-      <c r="C108" s="66"/>
-      <c r="D108" s="66"/>
-      <c r="E108" s="66"/>
-      <c r="F108" s="66"/>
-      <c r="G108" s="67"/>
-      <c r="H108" s="66"/>
-      <c r="I108" s="66"/>
-      <c r="J108" s="66"/>
-      <c r="K108" s="66"/>
-      <c r="L108" s="68" t="n">
+      <c r="B108" s="62"/>
+      <c r="C108" s="63"/>
+      <c r="D108" s="63"/>
+      <c r="E108" s="63"/>
+      <c r="F108" s="63"/>
+      <c r="G108" s="64"/>
+      <c r="H108" s="63"/>
+      <c r="I108" s="63"/>
+      <c r="J108" s="63"/>
+      <c r="K108" s="63"/>
+      <c r="L108" s="65" t="n">
         <f aca="false">K108*$D$25</f>
         <v>0</v>
       </c>
     </row>
     <row r="109" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B109" s="65"/>
-      <c r="C109" s="66"/>
-      <c r="D109" s="66"/>
-      <c r="E109" s="66"/>
-      <c r="F109" s="66"/>
-      <c r="G109" s="67"/>
-      <c r="H109" s="66"/>
-      <c r="I109" s="66"/>
-      <c r="J109" s="66"/>
-      <c r="K109" s="66"/>
-      <c r="L109" s="68" t="n">
+      <c r="B109" s="62"/>
+      <c r="C109" s="63"/>
+      <c r="D109" s="63"/>
+      <c r="E109" s="63"/>
+      <c r="F109" s="63"/>
+      <c r="G109" s="64"/>
+      <c r="H109" s="63"/>
+      <c r="I109" s="63"/>
+      <c r="J109" s="63"/>
+      <c r="K109" s="63"/>
+      <c r="L109" s="65" t="n">
         <f aca="false">K109*$D$25</f>
         <v>0</v>
       </c>
     </row>
     <row r="110" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B110" s="65"/>
-      <c r="C110" s="66"/>
-      <c r="D110" s="66"/>
-      <c r="E110" s="66"/>
-      <c r="F110" s="66"/>
-      <c r="G110" s="67"/>
-      <c r="H110" s="66"/>
-      <c r="I110" s="66"/>
-      <c r="J110" s="66"/>
-      <c r="K110" s="66"/>
-      <c r="L110" s="68" t="n">
+      <c r="B110" s="62"/>
+      <c r="C110" s="63"/>
+      <c r="D110" s="63"/>
+      <c r="E110" s="63"/>
+      <c r="F110" s="63"/>
+      <c r="G110" s="64"/>
+      <c r="H110" s="63"/>
+      <c r="I110" s="63"/>
+      <c r="J110" s="63"/>
+      <c r="K110" s="63"/>
+      <c r="L110" s="65" t="n">
         <f aca="false">K110*$D$25</f>
         <v>0</v>
       </c>
     </row>
     <row r="111" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B111" s="65"/>
-      <c r="C111" s="66"/>
-      <c r="D111" s="66"/>
-      <c r="E111" s="66"/>
-      <c r="F111" s="66"/>
-      <c r="G111" s="67"/>
-      <c r="H111" s="66"/>
-      <c r="I111" s="66"/>
-      <c r="J111" s="66"/>
-      <c r="K111" s="66"/>
-      <c r="L111" s="68" t="n">
+      <c r="B111" s="62"/>
+      <c r="C111" s="63"/>
+      <c r="D111" s="63"/>
+      <c r="E111" s="63"/>
+      <c r="F111" s="63"/>
+      <c r="G111" s="64"/>
+      <c r="H111" s="63"/>
+      <c r="I111" s="63"/>
+      <c r="J111" s="63"/>
+      <c r="K111" s="63"/>
+      <c r="L111" s="65" t="n">
         <f aca="false">K111*$D$25</f>
         <v>0</v>
       </c>
     </row>
     <row r="112" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B112" s="65"/>
-      <c r="C112" s="66"/>
-      <c r="D112" s="66"/>
-      <c r="E112" s="66"/>
-      <c r="F112" s="66"/>
-      <c r="G112" s="67"/>
-      <c r="H112" s="66"/>
-      <c r="I112" s="66"/>
-      <c r="J112" s="66"/>
-      <c r="K112" s="66"/>
-      <c r="L112" s="68" t="n">
+      <c r="B112" s="62"/>
+      <c r="C112" s="63"/>
+      <c r="D112" s="63"/>
+      <c r="E112" s="63"/>
+      <c r="F112" s="63"/>
+      <c r="G112" s="64"/>
+      <c r="H112" s="63"/>
+      <c r="I112" s="63"/>
+      <c r="J112" s="63"/>
+      <c r="K112" s="63"/>
+      <c r="L112" s="65" t="n">
         <f aca="false">K112*$D$25</f>
         <v>0</v>
       </c>
     </row>
     <row r="113" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B113" s="65"/>
-      <c r="C113" s="66"/>
-      <c r="D113" s="66"/>
-      <c r="E113" s="66"/>
-      <c r="F113" s="66"/>
-      <c r="G113" s="67"/>
-      <c r="H113" s="66"/>
-      <c r="I113" s="66"/>
-      <c r="J113" s="66"/>
-      <c r="K113" s="66"/>
-      <c r="L113" s="68" t="n">
+      <c r="B113" s="62"/>
+      <c r="C113" s="63"/>
+      <c r="D113" s="63"/>
+      <c r="E113" s="63"/>
+      <c r="F113" s="63"/>
+      <c r="G113" s="64"/>
+      <c r="H113" s="63"/>
+      <c r="I113" s="63"/>
+      <c r="J113" s="63"/>
+      <c r="K113" s="63"/>
+      <c r="L113" s="65" t="n">
         <f aca="false">K113*$D$25</f>
         <v>0</v>
       </c>
     </row>
     <row r="114" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B114" s="65"/>
-      <c r="C114" s="66"/>
-      <c r="D114" s="66"/>
-      <c r="E114" s="66"/>
-      <c r="F114" s="66"/>
-      <c r="G114" s="67"/>
-      <c r="H114" s="66"/>
-      <c r="I114" s="66"/>
-      <c r="J114" s="66"/>
-      <c r="K114" s="66"/>
-      <c r="L114" s="68" t="n">
+      <c r="B114" s="62"/>
+      <c r="C114" s="63"/>
+      <c r="D114" s="63"/>
+      <c r="E114" s="63"/>
+      <c r="F114" s="63"/>
+      <c r="G114" s="64"/>
+      <c r="H114" s="63"/>
+      <c r="I114" s="63"/>
+      <c r="J114" s="63"/>
+      <c r="K114" s="63"/>
+      <c r="L114" s="65" t="n">
         <f aca="false">K114*$D$25</f>
         <v>0</v>
       </c>
     </row>
     <row r="115" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B115" s="65"/>
-      <c r="C115" s="66"/>
-      <c r="D115" s="66"/>
-      <c r="E115" s="66"/>
-      <c r="F115" s="66"/>
-      <c r="G115" s="67"/>
-      <c r="H115" s="66"/>
-      <c r="I115" s="66"/>
-      <c r="J115" s="66"/>
-      <c r="K115" s="66"/>
-      <c r="L115" s="68" t="n">
+      <c r="B115" s="62"/>
+      <c r="C115" s="63"/>
+      <c r="D115" s="63"/>
+      <c r="E115" s="63"/>
+      <c r="F115" s="63"/>
+      <c r="G115" s="64"/>
+      <c r="H115" s="63"/>
+      <c r="I115" s="63"/>
+      <c r="J115" s="63"/>
+      <c r="K115" s="63"/>
+      <c r="L115" s="65" t="n">
         <f aca="false">K115*$D$25</f>
         <v>0</v>
       </c>
     </row>
     <row r="116" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B116" s="65"/>
-      <c r="C116" s="66"/>
-      <c r="D116" s="66"/>
-      <c r="E116" s="66"/>
-      <c r="F116" s="66"/>
-      <c r="G116" s="67"/>
-      <c r="H116" s="66"/>
-      <c r="I116" s="66"/>
-      <c r="J116" s="66"/>
-      <c r="K116" s="66"/>
-      <c r="L116" s="68" t="n">
+      <c r="B116" s="62"/>
+      <c r="C116" s="63"/>
+      <c r="D116" s="63"/>
+      <c r="E116" s="63"/>
+      <c r="F116" s="63"/>
+      <c r="G116" s="64"/>
+      <c r="H116" s="63"/>
+      <c r="I116" s="63"/>
+      <c r="J116" s="63"/>
+      <c r="K116" s="63"/>
+      <c r="L116" s="65" t="n">
         <f aca="false">K116*$D$25</f>
         <v>0</v>
       </c>
     </row>
     <row r="117" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B117" s="65"/>
-      <c r="C117" s="66"/>
-      <c r="D117" s="66"/>
-      <c r="E117" s="66"/>
-      <c r="F117" s="66"/>
-      <c r="G117" s="67"/>
-      <c r="H117" s="66"/>
-      <c r="I117" s="66"/>
-      <c r="J117" s="66"/>
-      <c r="K117" s="66"/>
-      <c r="L117" s="68" t="n">
+      <c r="B117" s="62"/>
+      <c r="C117" s="63"/>
+      <c r="D117" s="63"/>
+      <c r="E117" s="63"/>
+      <c r="F117" s="63"/>
+      <c r="G117" s="64"/>
+      <c r="H117" s="63"/>
+      <c r="I117" s="63"/>
+      <c r="J117" s="63"/>
+      <c r="K117" s="63"/>
+      <c r="L117" s="65" t="n">
         <f aca="false">K117*$D$25</f>
         <v>0</v>
       </c>
     </row>
     <row r="118" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B118" s="65"/>
-      <c r="C118" s="66"/>
-      <c r="D118" s="66"/>
-      <c r="E118" s="66"/>
-      <c r="F118" s="66"/>
-      <c r="G118" s="67"/>
-      <c r="H118" s="66"/>
-      <c r="I118" s="66"/>
-      <c r="J118" s="66"/>
-      <c r="K118" s="66"/>
-      <c r="L118" s="68" t="n">
+      <c r="B118" s="62"/>
+      <c r="C118" s="63"/>
+      <c r="D118" s="63"/>
+      <c r="E118" s="63"/>
+      <c r="F118" s="63"/>
+      <c r="G118" s="64"/>
+      <c r="H118" s="63"/>
+      <c r="I118" s="63"/>
+      <c r="J118" s="63"/>
+      <c r="K118" s="63"/>
+      <c r="L118" s="65" t="n">
         <f aca="false">K118*$D$25</f>
         <v>0</v>
       </c>
     </row>
     <row r="119" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B119" s="65"/>
-      <c r="C119" s="66"/>
-      <c r="D119" s="66"/>
-      <c r="E119" s="66"/>
-      <c r="F119" s="66"/>
-      <c r="G119" s="67"/>
-      <c r="H119" s="66"/>
-      <c r="I119" s="66"/>
-      <c r="J119" s="66"/>
-      <c r="K119" s="66"/>
-      <c r="L119" s="68" t="n">
+      <c r="B119" s="62"/>
+      <c r="C119" s="63"/>
+      <c r="D119" s="63"/>
+      <c r="E119" s="63"/>
+      <c r="F119" s="63"/>
+      <c r="G119" s="64"/>
+      <c r="H119" s="63"/>
+      <c r="I119" s="63"/>
+      <c r="J119" s="63"/>
+      <c r="K119" s="63"/>
+      <c r="L119" s="65" t="n">
         <f aca="false">K119*$D$25</f>
         <v>0</v>
       </c>
     </row>
     <row r="120" customFormat="false" ht="13.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B120" s="65"/>
-      <c r="C120" s="66"/>
-      <c r="D120" s="66"/>
-      <c r="E120" s="66"/>
-      <c r="F120" s="66"/>
-      <c r="G120" s="67"/>
-      <c r="H120" s="66"/>
-      <c r="I120" s="66"/>
-      <c r="J120" s="66"/>
-      <c r="K120" s="66"/>
-      <c r="L120" s="68" t="n">
+      <c r="B120" s="62"/>
+      <c r="C120" s="63"/>
+      <c r="D120" s="63"/>
+      <c r="E120" s="63"/>
+      <c r="F120" s="63"/>
+      <c r="G120" s="64"/>
+      <c r="H120" s="63"/>
+      <c r="I120" s="63"/>
+      <c r="J120" s="63"/>
+      <c r="K120" s="63"/>
+      <c r="L120" s="65" t="n">
         <f aca="false">K120*$D$25</f>
         <v>0</v>
       </c>
     </row>
     <row r="121" customFormat="false" ht="13.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B121" s="65"/>
-      <c r="C121" s="66"/>
-      <c r="D121" s="66"/>
-      <c r="E121" s="66"/>
-      <c r="F121" s="66"/>
-      <c r="G121" s="67"/>
-      <c r="H121" s="66"/>
-      <c r="I121" s="66"/>
-      <c r="J121" s="66"/>
-      <c r="K121" s="66"/>
-      <c r="L121" s="68" t="n">
+      <c r="B121" s="62"/>
+      <c r="C121" s="63"/>
+      <c r="D121" s="63"/>
+      <c r="E121" s="63"/>
+      <c r="F121" s="63"/>
+      <c r="G121" s="64"/>
+      <c r="H121" s="63"/>
+      <c r="I121" s="63"/>
+      <c r="J121" s="63"/>
+      <c r="K121" s="63"/>
+      <c r="L121" s="65" t="n">
         <f aca="false">K121*$D$25</f>
         <v>0</v>
       </c>
     </row>
     <row r="122" customFormat="false" ht="13.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B122" s="65"/>
-      <c r="C122" s="66"/>
-      <c r="D122" s="66"/>
-      <c r="E122" s="66"/>
-      <c r="F122" s="66"/>
-      <c r="G122" s="67"/>
-      <c r="H122" s="66"/>
-      <c r="I122" s="66"/>
-      <c r="J122" s="66"/>
-      <c r="K122" s="66"/>
-      <c r="L122" s="68" t="n">
+      <c r="B122" s="62"/>
+      <c r="C122" s="63"/>
+      <c r="D122" s="63"/>
+      <c r="E122" s="63"/>
+      <c r="F122" s="63"/>
+      <c r="G122" s="64"/>
+      <c r="H122" s="63"/>
+      <c r="I122" s="63"/>
+      <c r="J122" s="63"/>
+      <c r="K122" s="63"/>
+      <c r="L122" s="65" t="n">
         <f aca="false">K122*$D$25</f>
         <v>0</v>
       </c>
     </row>
     <row r="123" customFormat="false" ht="13.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B123" s="65"/>
-      <c r="C123" s="66"/>
-      <c r="D123" s="66"/>
-      <c r="E123" s="66"/>
-      <c r="F123" s="66"/>
-      <c r="G123" s="67"/>
-      <c r="H123" s="66"/>
-      <c r="I123" s="66"/>
-      <c r="J123" s="66"/>
-      <c r="K123" s="66"/>
-      <c r="L123" s="68" t="n">
+      <c r="B123" s="62"/>
+      <c r="C123" s="63"/>
+      <c r="D123" s="63"/>
+      <c r="E123" s="63"/>
+      <c r="F123" s="63"/>
+      <c r="G123" s="64"/>
+      <c r="H123" s="63"/>
+      <c r="I123" s="63"/>
+      <c r="J123" s="63"/>
+      <c r="K123" s="63"/>
+      <c r="L123" s="65" t="n">
         <f aca="false">K123*$D$25</f>
         <v>0</v>
       </c>
     </row>
     <row r="124" customFormat="false" ht="13.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B124" s="65"/>
-      <c r="C124" s="66"/>
-      <c r="D124" s="66"/>
-      <c r="E124" s="66"/>
-      <c r="F124" s="66"/>
-      <c r="G124" s="67"/>
-      <c r="H124" s="66"/>
-      <c r="I124" s="66"/>
-      <c r="J124" s="66"/>
-      <c r="K124" s="66"/>
-      <c r="L124" s="68" t="n">
+      <c r="B124" s="62"/>
+      <c r="C124" s="63"/>
+      <c r="D124" s="63"/>
+      <c r="E124" s="63"/>
+      <c r="F124" s="63"/>
+      <c r="G124" s="64"/>
+      <c r="H124" s="63"/>
+      <c r="I124" s="63"/>
+      <c r="J124" s="63"/>
+      <c r="K124" s="63"/>
+      <c r="L124" s="65" t="n">
         <f aca="false">K124*$D$25</f>
         <v>0</v>
       </c>
     </row>
     <row r="125" customFormat="false" ht="13.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B125" s="65"/>
-      <c r="C125" s="66"/>
-      <c r="D125" s="66"/>
-      <c r="E125" s="66"/>
-      <c r="F125" s="66"/>
-      <c r="G125" s="67"/>
-      <c r="H125" s="66"/>
-      <c r="I125" s="66"/>
-      <c r="J125" s="66"/>
-      <c r="K125" s="66"/>
-      <c r="L125" s="68" t="n">
+      <c r="B125" s="62"/>
+      <c r="C125" s="63"/>
+      <c r="D125" s="63"/>
+      <c r="E125" s="63"/>
+      <c r="F125" s="63"/>
+      <c r="G125" s="64"/>
+      <c r="H125" s="63"/>
+      <c r="I125" s="63"/>
+      <c r="J125" s="63"/>
+      <c r="K125" s="63"/>
+      <c r="L125" s="65" t="n">
         <f aca="false">K125*$D$25</f>
         <v>0</v>
       </c>
     </row>
     <row r="126" customFormat="false" ht="13.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B126" s="65"/>
-      <c r="C126" s="66"/>
-      <c r="D126" s="66"/>
-      <c r="E126" s="66"/>
-      <c r="F126" s="66"/>
-      <c r="G126" s="67"/>
-      <c r="H126" s="66"/>
-      <c r="I126" s="66"/>
-      <c r="J126" s="66"/>
-      <c r="K126" s="66"/>
-      <c r="L126" s="68" t="n">
+      <c r="B126" s="62"/>
+      <c r="C126" s="63"/>
+      <c r="D126" s="63"/>
+      <c r="E126" s="63"/>
+      <c r="F126" s="63"/>
+      <c r="G126" s="64"/>
+      <c r="H126" s="63"/>
+      <c r="I126" s="63"/>
+      <c r="J126" s="63"/>
+      <c r="K126" s="63"/>
+      <c r="L126" s="65" t="n">
         <f aca="false">K126*$D$25</f>
         <v>0</v>
       </c>
     </row>
     <row r="127" customFormat="false" ht="13.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B127" s="65"/>
-      <c r="C127" s="66"/>
-      <c r="D127" s="66"/>
-      <c r="E127" s="66"/>
-      <c r="F127" s="66"/>
-      <c r="G127" s="67"/>
-      <c r="H127" s="66"/>
-      <c r="I127" s="66"/>
-      <c r="J127" s="66"/>
-      <c r="K127" s="66"/>
-      <c r="L127" s="68" t="n">
+      <c r="B127" s="62"/>
+      <c r="C127" s="63"/>
+      <c r="D127" s="63"/>
+      <c r="E127" s="63"/>
+      <c r="F127" s="63"/>
+      <c r="G127" s="64"/>
+      <c r="H127" s="63"/>
+      <c r="I127" s="63"/>
+      <c r="J127" s="63"/>
+      <c r="K127" s="63"/>
+      <c r="L127" s="65" t="n">
         <f aca="false">K127*$D$25</f>
         <v>0</v>
       </c>
     </row>
     <row r="128" customFormat="false" ht="13.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B128" s="65"/>
-      <c r="C128" s="66"/>
-      <c r="D128" s="66"/>
-      <c r="E128" s="66"/>
-      <c r="F128" s="66"/>
-      <c r="G128" s="67"/>
-      <c r="H128" s="66"/>
-      <c r="I128" s="66"/>
-      <c r="J128" s="66"/>
-      <c r="K128" s="66"/>
-      <c r="L128" s="68" t="n">
+      <c r="B128" s="62"/>
+      <c r="C128" s="63"/>
+      <c r="D128" s="63"/>
+      <c r="E128" s="63"/>
+      <c r="F128" s="63"/>
+      <c r="G128" s="64"/>
+      <c r="H128" s="63"/>
+      <c r="I128" s="63"/>
+      <c r="J128" s="63"/>
+      <c r="K128" s="63"/>
+      <c r="L128" s="65" t="n">
         <f aca="false">K128*$D$25</f>
         <v>0</v>
       </c>

</xml_diff>

<commit_message>
R97 = n. m.
</commit_message>
<xml_diff>
--- a/central_unit/production_data/BOM_Central Unit for AgOpenGPS__Shenzhen2u .xlsx
+++ b/central_unit/production_data/BOM_Central Unit for AgOpenGPS__Shenzhen2u .xlsx
@@ -476,7 +476,7 @@
     <t xml:space="preserve">OSC-SMD_4P-L2.0-W1.6-BL</t>
   </si>
   <si>
-    <t xml:space="preserve">R97,R83,R43,R46,R101,R100</t>
+    <t xml:space="preserve">R83,R43,R46,R101,R100</t>
   </si>
   <si>
     <t xml:space="preserve">RALEC</t>
@@ -1525,9 +1525,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>4</xdr:col>
-      <xdr:colOff>922680</xdr:colOff>
+      <xdr:colOff>922320</xdr:colOff>
       <xdr:row>6</xdr:row>
-      <xdr:rowOff>96480</xdr:rowOff>
+      <xdr:rowOff>96120</xdr:rowOff>
     </xdr:to>
     <xdr:sp>
       <xdr:nvSpPr>
@@ -1536,8 +1536,8 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="1771560" y="133200"/>
-          <a:ext cx="2246400" cy="1036080"/>
+          <a:off x="1752480" y="133200"/>
+          <a:ext cx="2227320" cy="1035720"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -1703,9 +1703,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>2</xdr:col>
-      <xdr:colOff>577800</xdr:colOff>
+      <xdr:colOff>577440</xdr:colOff>
       <xdr:row>5</xdr:row>
-      <xdr:rowOff>129600</xdr:rowOff>
+      <xdr:rowOff>129240</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -1718,8 +1718,8 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="790200" y="123840"/>
-          <a:ext cx="1082880" cy="911160"/>
+          <a:off x="780840" y="123840"/>
+          <a:ext cx="1072800" cy="910800"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -1741,23 +1741,23 @@
   </sheetPr>
   <dimension ref="1:128"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="false" showRowColHeaders="true" showZeros="false" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A79" colorId="64" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="E103" activeCellId="0" sqref="E103"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="false" showRowColHeaders="true" showZeros="false" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A36" colorId="64" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="K56" activeCellId="0" sqref="K56"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.2"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="10.8010204081633"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="7.56122448979592"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="1" width="10.2602040816327"/>
-    <col collapsed="false" hidden="false" max="8" min="4" style="1" width="15.2551020408163"/>
-    <col collapsed="false" hidden="false" max="9" min="9" style="1" width="10.2602040816327"/>
-    <col collapsed="false" hidden="false" max="10" min="10" style="1" width="18.0867346938776"/>
-    <col collapsed="false" hidden="false" max="12" min="11" style="1" width="8.23469387755102"/>
-    <col collapsed="false" hidden="false" max="13" min="13" style="1" width="1.35204081632653"/>
-    <col collapsed="false" hidden="false" max="14" min="14" style="1" width="8.50510204081633"/>
-    <col collapsed="false" hidden="false" max="15" min="15" style="1" width="10.2602040816327"/>
-    <col collapsed="false" hidden="false" max="1025" min="16" style="1" width="8.50510204081633"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="10.6632653061225"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="7.4234693877551"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="1" width="10.1224489795918"/>
+    <col collapsed="false" hidden="false" max="8" min="4" style="1" width="15.1173469387755"/>
+    <col collapsed="false" hidden="false" max="9" min="9" style="1" width="10.1224489795918"/>
+    <col collapsed="false" hidden="false" max="10" min="10" style="1" width="17.8214285714286"/>
+    <col collapsed="false" hidden="false" max="12" min="11" style="1" width="8.10204081632653"/>
+    <col collapsed="false" hidden="false" max="13" min="13" style="1" width="1.21428571428571"/>
+    <col collapsed="false" hidden="false" max="14" min="14" style="1" width="8.36734693877551"/>
+    <col collapsed="false" hidden="false" max="15" min="15" style="1" width="10.1224489795918"/>
+    <col collapsed="false" hidden="false" max="1025" min="16" style="1" width="8.36734693877551"/>
   </cols>
   <sheetData>
     <row r="1" s="2" customFormat="true" ht="20.3" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -38417,7 +38417,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="55" customFormat="false" ht="30.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="55" customFormat="false" ht="30.55" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A55" s="61"/>
       <c r="B55" s="62" t="n">
         <v>24</v>
@@ -38445,7 +38445,7 @@
         <v>73</v>
       </c>
       <c r="K55" s="63" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="L55" s="65" t="n">
         <f aca="false">K55*$D$25</f>

</xml_diff>